<commit_message>
new choice for human eval, only take footnotes that actually are in the dev set (after filtering)
</commit_message>
<xml_diff>
--- a/evaluate/human_eval/evaluation_form_v1.xlsx
+++ b/evaluate/human_eval/evaluation_form_v1.xlsx
@@ -516,7 +516,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>11755_99</t>
+          <t>11755_104</t>
         </is>
       </c>
       <c r="C2" s="6" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="D2" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 99</t>
+          <t>Fussnote 104</t>
         </is>
       </c>
       <c r="E2" s="6" t="n"/>
@@ -537,17 +537,17 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dann sie seynt alle unnutze knecht,__99 haben alle gesundiget und manglen des preises, den gott an yhn haben soll [Röm 3, 23].</t>
+          <t>Paulus hab von der jungfrawschafft (on zweifel auch von der digamey) keyn gepott noch verpott des herren, geb wol davon seyn trewen rath__104.</t>
         </is>
       </c>
       <c r="D3" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1Kor 7, 25.</t>
         </is>
       </c>
       <c r="E3" s="7" t="n"/>
@@ -558,7 +558,7 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D4" s="8" t="inlineStr">
@@ -574,12 +574,12 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>Vgl. Lk 17, 10.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E5" s="7" t="n"/>
@@ -590,7 +590,7 @@
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D6" s="8" t="inlineStr">
@@ -606,17 +606,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13080_70</t>
+          <t>10052_38</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Ambrosius Blarer (Blaurer) / [Konstanz] an Heinrich Bullinger, 4. Oktober [1547]</t>
+          <t>[Heinrich Bullinger] / [Kappel am Albis] an [Anna Bullinger, geb. Adlischwyler], [Ende 1527 oder 1. Hälfte 1528]</t>
         </is>
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 70</t>
+          <t>Fussnote 38</t>
         </is>
       </c>
       <c r="E7" s="6" t="n"/>
@@ -632,7 +632,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Mitt unsern predigen und kirchenuͤbungen stets noch ymmerdaren gleich, und wie ich euch vormals geschriben.__70</t>
+          <t>Es ist ye gwüß, daß gott den eelichen stand hat ingesetzt, daß man ye damitt nitt sündet__38.</t>
         </is>
       </c>
       <c r="D8" s="7" t="inlineStr">
@@ -664,12 +664,12 @@
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
-          <t>Vgl. oben Z. .</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E10" s="7" t="n"/>
@@ -680,12 +680,12 @@
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1 Kor 7,2. 28. 36.</t>
         </is>
       </c>
       <c r="E11" s="8" t="n"/>
@@ -696,17 +696,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10495_30</t>
+          <t>12628_83</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>[Nikolaus Steiner] / [Zürich] an [Synode] / [Zürich], [vor 20. Oktober 1534]</t>
+          <t>Philipp von Hessen d.Ä., Simon Bing / Wechingen an Heinrich Bullinger, 12. September 1546</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 30</t>
+          <t>Fussnote 83</t>
         </is>
       </c>
       <c r="E12" s="6" t="n"/>
@@ -717,17 +717,17 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Unnd ist allso, wie ich gesechen han, das ich bißhar von aller mentschlicher hillf, radt unnd trost verlassen bin, unnd das zechen jar lang, unnd umb des vatterlands unnd voran gottes eer willen umb all min hab unnd guͦt kommen bin__30, das nit kleyn ist, unnd die vergangnen drü jar loblich unnd eerlich eyner gstifft gedienet hab umb 12 guldin uff hoffnung der gnaden, unnd aber keyn gnad nienen gespürt han, sonnder verschupft unnd verworfen bin, unnd aber so vyl jar unnd tag uff mir han, das ich zuͦ keyner arbeyt mee gschickt unnd vermüglich bin, dann ich gar nach der eltest predicant bin unnd dryßig unnd acht jar eerlich der kilchen gedienet han unnd mir keyn negligentz noch versumnus nie fürgehalten, so han ich nun rechtbrief unnd sigel an eynen herren von Eynsidlen durch sin amptman wellen lassen erfordren.</t>
+          <t>Auch lieber, besonder, als wir am 2. tag septembris den vheind, wie ir das aus unsern euch hirneben uberschickten verzeichnussen zu sehen hapt, so weidlich beschossenn, ist uns seidher des die gewisse kuntschafft zukommen, do wir desselben tags vortgetruckt__83, das wir was trefflichs gegen dem vheind ausgericht, unnd demselben großen abbruch gethan hattenn; wilchs aber an unser person nit gemangelt hat, sondern ist aus der ursachen bescheenn, dieweil der keyser an der statt Ingelstatt gelegen, unnd di zu seinem vortheil gehapt, haben ezlich dis bedencken getragen, das ime da nit viel abbruch, aber unserm volck woll großer schad vom geschuz het mugenn bescheen, wiewol dasselbe bedenckenn nit von ungutherzigen, sondern denen bescheen, wilchs ane zweivel auch trewlich unnd gutt gemeint.</t>
         </is>
       </c>
       <c r="D13" s="7" t="inlineStr">
         <is>
-          <t>Steiner verlor seine Habe als Pfarrer in Bünzen (s. Zürich StA, E II 1, 70), das er vor den anrückenden Truppen der V Orte fluchtartig verlassen mußte. Die katholischen Truppen richteten besonders in den verlassenen Häusern der reformierten Pfarrer große Zerstörungen an (s. Emil Schultz, Reformation und Gegenreformation in den Freien-Ämtern, Diss. phil. Basel, Zürich 1899, S. 90).</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E13" s="7" t="n"/>
@@ -738,12 +738,12 @@
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Siehe oben Anm. 53.</t>
         </is>
       </c>
       <c r="E14" s="8" t="n"/>
@@ -770,7 +770,7 @@
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
@@ -786,17 +786,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>12168_51</t>
+          <t>12552_17</t>
         </is>
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>Gervasius Schuler (Scholasticus) / Memmingen an Heinrich Bullinger, 23. März 1545</t>
+          <t>Ambrosius Blarer (Blaurer) / [Konstanz] an Heinrich Bullinger, 20. Juli 1546</t>
         </is>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 51</t>
+          <t>Fussnote 17</t>
         </is>
       </c>
       <c r="E17" s="6" t="n"/>
@@ -807,12 +807,12 @@
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Senatus auxit salarium, ut annuatim ducentos florenos habeam, zehen malter kernen oder zwenzig mutt sampt der bhaußung und bholtzung__51 gnugsamlich.</t>
+          <t>Das schreiben__17, davon ir mir vormals meldung gethon, ist mir noch nitt zuͦkommen.</t>
         </is>
       </c>
       <c r="D18" s="7" t="inlineStr">
@@ -828,12 +828,12 @@
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Brief Nr. 2493 vom 10. Juli, den Hans Rych überbringen sollte und dessen Empfang Blarer am 22. Juli mündlich und am 27. Juli schriftlich Bullinger gegenüber bestätigte; s. Nr. 2514,60-62.</t>
         </is>
       </c>
       <c r="E19" s="8" t="n"/>
@@ -844,7 +844,7 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D20" s="7" t="inlineStr">
@@ -860,12 +860,12 @@
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>bhaußung und bholtzung: Wohnung und Holzversorgung.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E21" s="8" t="n"/>
@@ -876,17 +876,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>10350_7</t>
+          <t>10348_20</t>
         </is>
       </c>
       <c r="C22" s="6" t="inlineStr">
         <is>
-          <t>Oswald Myconius (Geißhüsler) / Basel an Heinrich Bullinger, 23. Januar 1534</t>
+          <t>Ambrosius Blarer (Blaurer) / [Konstanz] an Heinrich Bullinger, 20. Januar 1534</t>
         </is>
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 7</t>
+          <t>Fussnote 20</t>
         </is>
       </c>
       <c r="E22" s="6" t="n"/>
@@ -897,17 +897,17 @@
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Harwiderumb schlecht imm Ferdinandus für ein herrschafft in Kemten in der Steurma[r]k__7, die wil der fürst von Wirtenberg ouch nitt, sonder er beharret mit sinem fürnemen sampt sinem bystand.</t>
+          <t>Des globens halber verglychte man sich in der ainung, unß wol lydelich, und das es die gaistlich gnanten ouch nachgeben; aber es sind der nebenzettel so vyl, das es sich gar stost, und ist im gleich das man vor ain kardannel, in unsern landen haben werd, dann die handlung zwyschen koniglicher majestat und hertzog Christoff von Wirtemberg will sich ouch nitt richten lassen__20».</t>
         </is>
       </c>
       <c r="D23" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>König Ferdinand und Christoph von Württemberg einigten sich nicht, vgl. unten Z. 77-81 und Wille 120-130. 137f. 141-144.</t>
         </is>
       </c>
       <c r="E23" s="7" t="n"/>
@@ -918,12 +918,12 @@
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>Ein Kemten in der Steiermark ließ sich nicht nachweisen (aus «Kernten» verschrieben?); vgl. oben S. 48, Anm. 60.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E24" s="8" t="n"/>
@@ -934,7 +934,7 @@
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D25" s="7" t="inlineStr">
@@ -950,7 +950,7 @@
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
@@ -966,17 +966,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>13141_19</t>
+          <t>10368_11</t>
         </is>
       </c>
       <c r="C27" s="6" t="inlineStr">
         <is>
-          <t>[Ambrosius Blarer (Blaurer)] / [Konstanz] an Heinrich Bullinger, [zwischen dem 9. und 13. Dezember 1547]</t>
+          <t>Hans (I.) Vogler / St. Gallen an Heinrich Bullinger, 11. März 1534</t>
         </is>
       </c>
       <c r="D27" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 19</t>
+          <t>Fussnote 11</t>
         </is>
       </c>
       <c r="E27" s="6" t="n"/>
@@ -987,12 +987,12 @@
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Habend unsern herren anzögt, wie inen auch ain mandat zuͦkommen seye,__19 etc., ain nachpurlichs mittlyden gebärdet, und das inen laid seye, das sy sölichs thain muͤssind und sich kainswegs wissind ausszeschlöffen.</t>
+          <t>Witer hab gmeltem Toman der statschriber zuͦ Lindow mit fröden gsagt, wie im sin schwecher von Ougspurg, der grichtschriber, schribe, daß ain rat Ougspurg jetz 14 tag heftig und streng ghandlett, abzuͦstellen den bapsthum by inen, und syge hüt mitwoch 14 tag verschinen komen uff ain gmain oder grossen radt__11.</t>
         </is>
       </c>
       <c r="D28" s="7" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
@@ -1024,12 +1024,12 @@
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D30" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der Große Rat trat am 4. März zusammen. Am 6. März überbrachte eine Delegation der beiden Räte dem Domkapitel ein Schriftstück, in welchem der Wunsch nach einem Religionsgespräch geäußert wurde, s. Roth II 155f; Wolfgang Musculus an Blarer, 29. März 1534 (Blarer BW I 479f).</t>
         </is>
       </c>
       <c r="E30" s="7" t="n"/>
@@ -1040,12 +1040,12 @@
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Das entsprechende kaiserliche, an die Lindauer gerichtete Verbot datiert vom 3. November; s. Wolfart, aaO, S. 17, Nr. XXV. Die Lindauer versuchten also tatsächlich lange, wenn auch vergebens, das kaiserliche Verbot zu umgehen oder rückgängig zu machen. - Auch den Überlingern wurden Geschäfte mit Konstanz verboten; s. Nr. 3089,.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E31" s="8" t="n"/>
@@ -1056,17 +1056,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12453_78</t>
+          <t>12544_21</t>
         </is>
       </c>
       <c r="C32" s="6" t="inlineStr">
         <is>
-          <t>Johannes Haller d.J. / Augsburg an Heinrich Bullinger, 1. April 1546</t>
+          <t>Johannes Haab / Baden an Heinrich Bullinger, 12. Juli 1546</t>
         </is>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 78</t>
+          <t>Fussnote 21</t>
         </is>
       </c>
       <c r="E32" s="6" t="n"/>
@@ -1077,12 +1077,12 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Undt als der Joͤrg amm fritag wider herus gefaren ist undt gen Pethmes__78 kommen, da hatt er den poͤßwicht selb dritt zum metzger imm wirtshus gefunden.</t>
+          <t>Hand zu wordt,__21 sy habind niemand imm feld, wiewol wir auch gar nüt willens sind, niemand abzemanenn.</t>
         </is>
       </c>
       <c r="D33" s="7" t="inlineStr">
@@ -1098,12 +1098,12 @@
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Pöttmes, ca. 30 km nördlich von Augsburg.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E34" s="8" t="n"/>
@@ -1114,12 +1114,12 @@
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D35" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Hand zu wordt: Sie geben vor.</t>
         </is>
       </c>
       <c r="E35" s="7" t="n"/>
@@ -1130,7 +1130,7 @@
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D36" s="8" t="inlineStr">
@@ -1146,17 +1146,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>11503_171</t>
+          <t>11755_169</t>
         </is>
       </c>
       <c r="C37" s="6" t="inlineStr">
         <is>
-          <t>Joachim Vadian (von Watt) / St. Gallen an Heinrich Bullinger, 8. Februar 1541</t>
+          <t>Johannes Lening / Melsungen an Heinrich Bullinger, 16. Januar 1543</t>
         </is>
       </c>
       <c r="D37" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 171</t>
+          <t>Fussnote 169</t>
         </is>
       </c>
       <c r="E37" s="6" t="n"/>
@@ -1167,12 +1167,12 @@
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Disß alles ist geschechen und geben zuͦ Zürich im zechenden jar unsers kayserthumbs, der römer zinß zal 13, gezelt nach der geburdt Christi achthunderundzechen__171.</t>
+          <t>Wilchs du selbst must bekennen, wenn du dich erinnerst deynes buchleyns Vom eynigen, ewigen testament,__169 item deyner dialogen widder die widdertauffer, wie du daselbst handelst den locum: „Mutuum date nihil inde sperantes“ [Lk 6, 35], was du fur eyn underscheit zwischen dem gesatze und der sunden, und wie du drey grados gottlicher gepott machest und wilt nit, das man die christen nach dem gesatze (dann nach dem gesatze seyen wir allzumal sunder), sonder nach der gnade und glauben schetzen und erkennen soll.</t>
         </is>
       </c>
       <c r="D38" s="7" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D40" s="7" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="D41" s="8" t="inlineStr">
         <is>
-          <t>Die Indiktion stimmt nicht mit Herrscher- und Inkarnationsjahr überein. ZUB XIII, Nr. 121b/130a datiert die ursprüngliche Urkunde auf den 12. September 874 oder 876-887. Zur Datierungsproblematik vgl. ebd. und Steiner, aaO, S. 53-57. Bullinger erörtert die Datierung im Anschluss an seine Abschrift der lateinischen Urkunde in Zürich StA, EH II 451, 17f.</t>
+          <t>HBBibl I 54; vgl. oben Anm. 39.</t>
         </is>
       </c>
       <c r="E41" s="8" t="n"/>
@@ -1236,17 +1236,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>12824_51</t>
+          <t>12453_98</t>
         </is>
       </c>
       <c r="C42" s="6" t="inlineStr">
         <is>
-          <t>[Ambrosius Blarer (Blaurer)] / [Konstanz] an [Heinrich Bullinger], 27. Januar 1547</t>
+          <t>Johannes Haller d.J. / Augsburg an Heinrich Bullinger, 1. April 1546</t>
         </is>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 51</t>
+          <t>Fussnote 98</t>
         </is>
       </c>
       <c r="E42" s="6" t="n"/>
@@ -1257,17 +1257,17 @@
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Achte, er seye nunmehr gewisslich zuͦ Ulm.__51</t>
+          <t>Da sindt si beidt die stegen abgsprungen zum hus undt der statt hinus, undt wider uff ire roß gsessen undt darvon gerent__98.</t>
         </is>
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>Er traf am 25. Januar in Ulm ein; s. Nr. 2754, Anm. 18.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E43" s="7" t="n"/>
@@ -1310,12 +1310,12 @@
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D46" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. Lang, aaO, f. Biij,r.-v.; und [Enzinas], aaO, S. 137-142, wo das Ganze noch ausführlicher geschildert wird.</t>
         </is>
       </c>
       <c r="E46" s="8" t="n"/>
@@ -1326,17 +1326,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>12552_73</t>
+          <t>12982_3</t>
         </is>
       </c>
       <c r="C47" s="6" t="inlineStr">
         <is>
-          <t>Ambrosius Blarer (Blaurer) / [Konstanz] an Heinrich Bullinger, 20. Juli 1546</t>
+          <t>Sebastian Schertlin / Konstanz an Heinrich Bullinger, 28. Juni 1547</t>
         </is>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 73</t>
+          <t>Fussnote 3</t>
         </is>
       </c>
       <c r="E47" s="6" t="n"/>
@@ -1347,17 +1347,17 @@
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Von dem vorstraich__73 waist man noch nitt under den unseren, was es ist und was er maint.</t>
+          <t>Gunstiger unnd vertrauter lieber her, meister Henrich, zöiger diser, her Gabriel Arnolt von Rornfels__3, meines gnedigen hern hertzog Ott Henrichs pfaltzgrafen rentmaister und dess pfaltzgrafen Friderichs churfurstenn, etc., ratt, ain rechter liebhaber dess wort gottes unnd von desselben wegen jetzunder auch, gleich so wol als ich, vertribner, dweil er also herumb zeucht, die weil zu vertreibenn, und willens, die schöne statt Zurich zu besichtigenn, hat mich gepettenn, ime ain kuntschafft zu machen, damit er möchte die statt und allerlai schons wesens zusehen.</t>
         </is>
       </c>
       <c r="D48" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Rohrenfels (Lkr. Neuburg-Schrobenhausen), südlich von Neuburg a.d. Donau.</t>
         </is>
       </c>
       <c r="E48" s="7" t="n"/>
@@ -1368,7 +1368,7 @@
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D49" s="8" t="inlineStr">
@@ -1384,12 +1384,12 @@
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D50" s="7" t="inlineStr">
         <is>
-          <t>Offensive. - Bullinger wird sich wohl nochmals (s. schon Nr. 2496,76-78) nach dem Zug von Landgraf Philipp von Hessen in Richtung  Süddeutschland erkundigt haben.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E50" s="7" t="n"/>
@@ -1400,7 +1400,7 @@
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D51" s="8" t="inlineStr">
@@ -1416,17 +1416,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>13093_10</t>
+          <t>12500_58</t>
         </is>
       </c>
       <c r="C52" s="6" t="inlineStr">
         <is>
-          <t>Sigismund Stier (Taurus) / Basel an [Heinrich Bullinger], 17. Oktober 1547</t>
+          <t>Georg Frölich (Laetus) / [Augsburg] an Heinrich Bullinger, 3. Juni 1546</t>
         </is>
       </c>
       <c r="D52" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 10</t>
+          <t>Fussnote 58</t>
         </is>
       </c>
       <c r="E52" s="6" t="n"/>
@@ -1437,17 +1437,17 @@
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Und dwyll die bemelten zway schryben, er hieher gebracht, hochgedachten mynen gnedigen hern, etc., gar nit berüren, ist ime sein bottenlon, dass er dan ungestümelich und mit ungepürlichen worthen gefordert, alhie nit entricht worden (wiewol er syn gnaden vorn heuptern alhie desselbenn verclagt), aber ime der beschaidt worden: Er möcht wol ein irrigen kopf haben; hab sich unbillich beklagt; soll die antwort von synen gnaden nemmen, sampt einer bekanthnus__10 von dero gnaden cantzley, daß ime sein bottenlon noch ußstehe, und hinziehen!</t>
+          <t>So haben wir den brunschwigischen krieg,__58 die recusation des chamergerichts, der concilien und die gantz religion, deren kains erortert ist.</t>
         </is>
       </c>
       <c r="D53" s="7" t="inlineStr">
         <is>
-          <t>Bescheinigung. - Damit ist das vorliegende Schreiben der gräflichen Kanzlei gemeint.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E53" s="7" t="n"/>
@@ -1458,7 +1458,7 @@
     <row r="54">
       <c r="B54" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D54" s="8" t="inlineStr">
@@ -1474,7 +1474,7 @@
     <row r="55">
       <c r="B55" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D55" s="7" t="inlineStr">
@@ -1490,12 +1490,12 @@
     <row r="56">
       <c r="B56" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D56" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Siehe dazu Nr. 2452, Anm. 2.</t>
         </is>
       </c>
       <c r="E56" s="8" t="n"/>
@@ -1506,17 +1506,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>12507_8</t>
+          <t>13141_38</t>
         </is>
       </c>
       <c r="C57" s="6" t="inlineStr">
         <is>
-          <t>Georg Frölich (Laetus) / [Augsburg] an Heinrich Bullinger, 13. Juni 1546</t>
+          <t>[Ambrosius Blarer (Blaurer)] / [Konstanz] an Heinrich Bullinger, [zwischen dem 9. und 13. Dezember 1547]</t>
         </is>
       </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 8</t>
+          <t>Fussnote 38</t>
         </is>
       </c>
       <c r="E57" s="6" t="n"/>
@@ -1527,12 +1527,12 @@
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Uber wene es angesehen__8, des konnen wir nit wissen.</t>
+          <t>Ich schick euch ain brieff von ainem vertrauwten in des alten churfursten von Sachsen cantzley, der mir ouch daby in ainem ingelegten zeddtel under anderm schrei[bt],__38 das hertzog Moritz hinwegh seye auss Augspurg.</t>
         </is>
       </c>
       <c r="D58" s="7" t="inlineStr">
@@ -1548,7 +1548,7 @@
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D59" s="8" t="inlineStr">
@@ -1564,7 +1564,7 @@
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D60" s="7" t="inlineStr">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="D61" s="8" t="inlineStr">
         <is>
-          <t>Uber wene es angesehen: Auf wen sie es damit abgesehen haben.</t>
+          <t>Vermutlich waren es diese beiden Dokumente, die Blarer am 26. Dezember zurückverlangte; s. oben .</t>
         </is>
       </c>
       <c r="E61" s="8" t="n"/>
@@ -1596,17 +1596,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>12425_40</t>
+          <t>10729_30</t>
         </is>
       </c>
       <c r="C62" s="6" t="inlineStr">
         <is>
-          <t>Peter Simler (Simmler) / [Kappel am Albis] an Heinrich Bullinger, 12. März 1546</t>
+          <t>Berchtold Haller / [Bern] an Heinrich Bullinger, 29. November [1535]</t>
         </is>
       </c>
       <c r="D62" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 40</t>
+          <t>Fussnote 30</t>
         </is>
       </c>
       <c r="E62" s="6" t="n"/>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Unnd do mine heren von rädten unnd burgern im 39. jar hinüber gan Cappel schicktent m. Müller, juncker Hans Edlibach__40 unnd amman Köchly, unnd ich inen die ordnung miner diensten unnd der gantzen hushallt anzeugt, hattend sy ein guͦt vernuͤgen.</t>
+          <t>Da sind unser botten gsin, habend die Berner knecht allein heim gmant, dann unser ordnung der reisglöffen semlichs fordret__30.</t>
         </is>
       </c>
       <c r="D63" s="7" t="inlineStr">
@@ -1638,12 +1638,12 @@
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D64" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Seit 1529 bzw. 1530 galt in Bern ein strenges Pensionen- und Reislaufverbot (SSRQ Bern I 11 362-368, vgl. Z XI 480, Anm. 4).</t>
         </is>
       </c>
       <c r="E64" s="8" t="n"/>
@@ -1654,12 +1654,12 @@
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D65" s="7" t="inlineStr">
         <is>
-          <t>Edlibach war damals offensichtlich Rechenherr; vgl. Fabian, Räte 510.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E65" s="7" t="n"/>
@@ -1686,17 +1686,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>12430_18</t>
+          <t>13141_11</t>
         </is>
       </c>
       <c r="C67" s="6" t="inlineStr">
         <is>
-          <t>Heinrich Bullinger / [Zürich] an Ambrosius Blarer (Blaurer), 18. März 1546</t>
+          <t>[Ambrosius Blarer (Blaurer)] / [Konstanz] an Heinrich Bullinger, [zwischen dem 9. und 13. Dezember 1547]</t>
         </is>
       </c>
       <c r="D67" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 18</t>
+          <t>Fussnote 11</t>
         </is>
       </c>
       <c r="E67" s="6" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Es kumpt ein red uß Franckrych, der koͤnig schick ein reysigen züg in das Pemondt, und werde Morellus herus gen Solenthurn__18 kummen mitt gaͤllt.</t>
+          <t>Des ehhandels halber beger ich von euch zuͦ vernemen, diewyl die personen im Turgöw sesshafft sind, davon ich euch geschriben habe, wie die guͦt tocht[er] vom gesellen, irem vetter, geschwengert seye, ob sich ewere herren zuͦ Zürich iren annemmen und uff fuͤrpitt, etc., mitt inen dispensieren und sy zuͦsamen lass[en] oder zuͦ kirchen gon gestatten wurden, und wann es ewere herren bewilligeten[d], ob sy darnach der anderen aidgnossen__11  halber im Turgöw belyben möchten.</t>
         </is>
       </c>
       <c r="D68" s="7" t="inlineStr">
@@ -1728,12 +1728,12 @@
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D69" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die katholischen Orte, die mit Zürich den Thurgau verwalteten.</t>
         </is>
       </c>
       <c r="E69" s="8" t="n"/>
@@ -1744,7 +1744,7 @@
     <row r="70">
       <c r="B70" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D70" s="7" t="inlineStr">
@@ -1760,12 +1760,12 @@
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D71" s="8" t="inlineStr">
         <is>
-          <t>Solothurn, Sitz des französischen Gesandten in der Schweiz.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E71" s="8" t="n"/>
@@ -1776,17 +1776,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>12500_30</t>
+          <t>12671_15</t>
         </is>
       </c>
       <c r="C72" s="6" t="inlineStr">
         <is>
-          <t>Georg Frölich (Laetus) / [Augsburg] an Heinrich Bullinger, 3. Juni 1546</t>
+          <t>Johannes Gast / Basel an Heinrich Bullinger, 14. Oktober 1546</t>
         </is>
       </c>
       <c r="D72" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 30</t>
+          <t>Fussnote 15</t>
         </is>
       </c>
       <c r="E72" s="6" t="n"/>
@@ -1797,12 +1797,12 @@
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Vom reichstag zw Regennspurg__30 kan ich nichts guts schreiben.</t>
+          <t>2. Oder aliud habet consilium: Er understadt, durch das wirtembergisch landt zuͦ ziehen, oder den weg ziehen, den die Niderlender heruff sindt zogen,__15 probant zuͦ fynden im wirtzburgischen oder bombergischen bistomen.</t>
         </is>
       </c>
       <c r="D73" s="7" t="inlineStr">
@@ -1818,12 +1818,12 @@
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D74" s="8" t="inlineStr">
         <is>
-          <t>Der Regensburger Reichstag, der am 5. Juni eröffnet werden sollte; s. HBBW XVI 97, Anm. 3.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E74" s="8" t="n"/>
@@ -1834,7 +1834,7 @@
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D75" s="7" t="inlineStr">
@@ -1850,12 +1850,12 @@
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D76" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Zu dieser Route des niederländischen Heeres unter Maximilian von Egmont, Graf von Büren, auf dem Weg zum kaiserlichen Lager s. HBBW XVII 415, Anm. 43.</t>
         </is>
       </c>
       <c r="E76" s="8" t="n"/>
@@ -1866,17 +1866,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>10287_30</t>
+          <t>13080_68</t>
         </is>
       </c>
       <c r="C77" s="6" t="inlineStr">
         <is>
-          <t>Berchtold Haller / Bern an Heinrich Bullinger, 25. August 1533</t>
+          <t>Ambrosius Blarer (Blaurer) / [Konstanz] an Heinrich Bullinger, 4. Oktober [1547]</t>
         </is>
       </c>
       <c r="D77" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 30</t>
+          <t>Fussnote 68</t>
         </is>
       </c>
       <c r="E77" s="6" t="n"/>
@@ -1887,12 +1887,12 @@
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Er welt sich gern hie niderlassen; gat uff hüt für rat__30, nescio successum.</t>
+          <t>Gewisß ists, das man gar sittsam mitt andern sachen handlen und nieman hochen__68 gern verbittern wirt, byß man vorhin den willen erlangt in denen sachen, die kai. m[ajesta]ten am nechsten diser zeyt angelegen.</t>
         </is>
       </c>
       <c r="D78" s="7" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="79">
       <c r="B79" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D79" s="8" t="inlineStr">
@@ -1924,12 +1924,12 @@
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D80" s="7" t="inlineStr">
         <is>
-          <t>geht heute vor den Rat.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E80" s="7" t="n"/>
@@ -1940,12 +1940,12 @@
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D81" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>nieman hochen: keine hochrangige Persönlichkeit.</t>
         </is>
       </c>
       <c r="E81" s="8" t="n"/>
@@ -1956,17 +1956,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>12671_14</t>
+          <t>13141_20</t>
         </is>
       </c>
       <c r="C82" s="6" t="inlineStr">
         <is>
-          <t>Johannes Gast / Basel an Heinrich Bullinger, 14. Oktober 1546</t>
+          <t>[Ambrosius Blarer (Blaurer)] / [Konstanz] an Heinrich Bullinger, [zwischen dem 9. und 13. Dezember 1547]</t>
         </is>
       </c>
       <c r="D82" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 14</t>
+          <t>Fussnote 20</t>
         </is>
       </c>
       <c r="E82" s="6" t="n"/>
@@ -1982,12 +1982,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2. Oder aliud habet consilium: Er understadt, durch das wirtembergisch landt zuͦ ziehen, oder den weg ziehen, den die Niderlender heruff__14 sindt zogen, probant zuͦ fynden im wirtzburgischen oder bombergischen bistomen.</t>
+          <t>Habend unsern herren anzögt, wie inen auch ain mandat zuͦkommen seye, etc., ain nachpurlichs mittlyden gebärdet__20, und das inen laid seye, das sy sölichs thain muͤssind und sich kainswegs wissind ausszeschlöffen.</t>
         </is>
       </c>
       <c r="D83" s="7" t="inlineStr">
         <is>
-          <t>d.h. in Richtung Süden.</t>
+          <t>ain mittlyden gebärdet: Anteilnahme bekundet.</t>
         </is>
       </c>
       <c r="E83" s="7" t="n"/>
@@ -2046,17 +2046,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>10368_7</t>
+          <t>12671_26</t>
         </is>
       </c>
       <c r="C87" s="6" t="inlineStr">
         <is>
-          <t>Hans (I.) Vogler / St. Gallen an Heinrich Bullinger, 11. März 1534</t>
+          <t>Johannes Gast / Basel an Heinrich Bullinger, 14. Oktober 1546</t>
         </is>
       </c>
       <c r="D87" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 7</t>
+          <t>Fussnote 26</t>
         </is>
       </c>
       <c r="E87" s="6" t="n"/>
@@ -2067,12 +2067,12 @@
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Witer hab gmeltem Toman der statschriber__7 zuͦ Lindow mit fröden gsagt, wie im sin schwecher von Ougspurg, der grichtschriber, schribe, daß ain rat Ougspurg jetz 14 tag heftig und streng ghandlett, abzuͦstellen den bapsthum by inen, und syge hüt mitwoch 14 tag verschinen komen uff ain gmain oder grossen radt.</t>
+          <t>Den hat sin schweher daniden__26 lassen vergraben (repugnantibus quibusdam bonis viris) mit kertzen, wiehwasser und luten, herlich gnuͦg.</t>
         </is>
       </c>
       <c r="D88" s="7" t="inlineStr">
@@ -2088,12 +2088,12 @@
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D89" s="8" t="inlineStr">
         <is>
-          <t>Anton Schmölz (Schmeltz).</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E89" s="8" t="n"/>
@@ -2104,12 +2104,12 @@
     <row r="90">
       <c r="B90" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D90" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>dort, nördlich von Basel.</t>
         </is>
       </c>
       <c r="E90" s="7" t="n"/>
@@ -2120,7 +2120,7 @@
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D91" s="8" t="inlineStr">
@@ -2136,17 +2136,17 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>12561_25</t>
+          <t>12879_10</t>
         </is>
       </c>
       <c r="C92" s="6" t="inlineStr">
         <is>
-          <t>Ambrosius Blarer (Blaurer) / [Konstanz] an Heinrich Bullinger, 27. Juli 1546</t>
+          <t>Gotthard Richmut / [Zürich] an Heinrich Bullinger, [s.d.]</t>
         </is>
       </c>
       <c r="D92" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 25</t>
+          <t>Fussnote 10</t>
         </is>
       </c>
       <c r="E92" s="6" t="n"/>
@@ -2157,17 +2157,17 @@
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Schreibt mir der burgermaister Herrbrot von Augsp[urg], des diener uff sontag__25 by mir gewesen.</t>
+          <t>Und aber ir hand es nit darby lan pliben und meister Andressen gen 4 batzen: Soͤlly__10 fur uch gaben.</t>
         </is>
       </c>
       <c r="D93" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>(Er) solle (sie).</t>
         </is>
       </c>
       <c r="E93" s="7" t="n"/>
@@ -2178,7 +2178,7 @@
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D94" s="8" t="inlineStr">
@@ -2194,7 +2194,7 @@
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D95" s="7" t="inlineStr">
@@ -2210,12 +2210,12 @@
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D96" s="8" t="inlineStr">
         <is>
-          <t>25. Juli.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E96" s="8" t="n"/>
@@ -2226,17 +2226,17 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>12743_70</t>
+          <t>10368_10</t>
         </is>
       </c>
       <c r="C97" s="6" t="inlineStr">
         <is>
-          <t>[Ambrosius Blarer (Blaurer)] / [Konstanz] an [Heinrich Bullinger], 27. November 1546</t>
+          <t>Hans (I.) Vogler / St. Gallen an Heinrich Bullinger, 11. März 1534</t>
         </is>
       </c>
       <c r="D97" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 70</t>
+          <t>Fussnote 10</t>
         </is>
       </c>
       <c r="E97" s="6" t="n"/>
@@ -2247,17 +2247,17 @@
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Item ettlich sagen, wie die Hessen und Seestett schicken dem churfursten__70 vyl volck zuͦ".</t>
+          <t>Witer hab gmeltem Toman der statschriber zuͦ Lindow mit fröden gsagt, wie im sin schwecher von Ougspurg, der grichtschriber, schribe, daß ain rat Ougspurg jetz 14 tag heftig und streng ghandlett, abzuͦstellen den bapsthum by inen, und syge hüt mitwoch 14 tag verschinen__10 komen uff ain gmain oder grossen radt.</t>
         </is>
       </c>
       <c r="D98" s="7" t="inlineStr">
         <is>
-          <t>Johann Friedrich I. von Sachsen.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E98" s="7" t="n"/>
@@ -2268,7 +2268,7 @@
     <row r="99">
       <c r="B99" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D99" s="8" t="inlineStr">
@@ -2300,12 +2300,12 @@
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D101" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>vor 14 Tagen.</t>
         </is>
       </c>
       <c r="E101" s="8" t="n"/>
@@ -2316,17 +2316,17 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>10870_6</t>
+          <t>10172_2</t>
         </is>
       </c>
       <c r="C102" s="6" t="inlineStr">
         <is>
-          <t>Heinrich Bullinger / [Zürich] an Kaspar Megander (Großmann), 27. Mai 1536</t>
+          <t>Gervasius Schuler (Scholasticus) / Basel an Heinrich Bullinger, 4. Oktober 1532</t>
         </is>
       </c>
       <c r="D102" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 6</t>
+          <t>Fussnote 2</t>
         </is>
       </c>
       <c r="E102" s="6" t="n"/>
@@ -2337,12 +2337,12 @@
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Societas regum Aegypti et Assyriorum nunquam bene cessit Israeli__6.</t>
+          <t>Carnis internitionem spiritus alimentum esse__2 in dies experior.</t>
         </is>
       </c>
       <c r="D103" s="7" t="inlineStr">
@@ -2358,7 +2358,7 @@
     <row r="104">
       <c r="B104" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D104" s="8" t="inlineStr">
@@ -2374,12 +2374,12 @@
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D105" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1 Kor 5,5.</t>
         </is>
       </c>
       <c r="E105" s="7" t="n"/>
@@ -2390,12 +2390,12 @@
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D106" s="8" t="inlineStr">
         <is>
-          <t>Vgl. z. B. Hos 7, 11f; 12, 2f.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E106" s="8" t="n"/>
@@ -2406,17 +2406,17 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>11755_17</t>
+          <t>11012_3</t>
         </is>
       </c>
       <c r="C107" s="6" t="inlineStr">
         <is>
-          <t>Johannes Lening / Melsungen an Heinrich Bullinger, 16. Januar 1543</t>
+          <t>Oswald Myconius (Geißhüsler) / Basel an Heinrich Bullinger, 14. März 1537</t>
         </is>
       </c>
       <c r="D107" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 17</t>
+          <t>Fussnote 3</t>
         </is>
       </c>
       <c r="E107" s="6" t="n"/>
@@ -2427,12 +2427,12 @@
     <row r="108">
       <c r="B108" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Quando Christus non novus legislator, non severus exactor, sed gratię conciliator, immo gratię plenus fuerit apostolique non litterę, sed spiritus ministri extiterint__17.</t>
+          <t>Per me abundet quisque in sensu suo__3; nam postquam Leo scribit: "Feremus Bucerum; tantum non cogite, ut subscribamus, tantum ne tot literis irritetis patientiam nostram" - et nobis tamen nihil tale in mentem venit; nam utrum cogere an fraterne monere voluerimus, literę nostrę satis, puto, testantur.</t>
         </is>
       </c>
       <c r="D108" s="7" t="inlineStr">
@@ -2448,12 +2448,12 @@
     <row r="109">
       <c r="B109" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D109" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. Röm 14, 5.</t>
         </is>
       </c>
       <c r="E109" s="8" t="n"/>
@@ -2480,12 +2480,12 @@
     <row r="111">
       <c r="B111" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D111" s="8" t="inlineStr">
         <is>
-          <t>Vgl. 2Kor 3, 6.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E111" s="8" t="n"/>
@@ -2496,17 +2496,17 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10417_1</t>
+          <t>10498_29</t>
         </is>
       </c>
       <c r="C112" s="6" t="inlineStr">
         <is>
-          <t>s.n. / Basel an Heinrich Bullinger / [Zürich], 25. Mai 1534</t>
+          <t>Heinrich Bullinger / [Zürich] an Ambrosius Blarer (Blaurer), [22. Oktober 1534]</t>
         </is>
       </c>
       <c r="D112" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 1</t>
+          <t>Fussnote 29</t>
         </is>
       </c>
       <c r="E112" s="6" t="n"/>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Non vos praeterit, fratres in domino charissimi, Myconium nostrum non ita multo ante scripsisse ad vos__1, si quem sciretis, qui posset in evangelii negocio prodesse nobis, indicaretis.</t>
+          <t>Caeterum nullo affectu aut praeiuditio__29 haec scribimus, qui optima quaeque speramus, maxime cum tu, Ambrosi, una cum Grynaeo nostro, sacratissima deo et sanctae concordiae dicata pectora, intelligatis, quantum hic nos conari, anniti laborareque conveniat.</t>
         </is>
       </c>
       <c r="D113" s="7" t="inlineStr">
@@ -2575,7 +2575,7 @@
       </c>
       <c r="D116" s="8" t="inlineStr">
         <is>
-          <t>Oben Nr. 359, bes. S. 134, 40-43.</t>
+          <t>1 Tim 5, 21.</t>
         </is>
       </c>
       <c r="E116" s="8" t="n"/>
@@ -2586,17 +2586,17 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>12770_77</t>
+          <t>11725_28</t>
         </is>
       </c>
       <c r="C117" s="6" t="inlineStr">
         <is>
-          <t>Johannes Haller d.J. / Augsburg an Heinrich Bullinger, 23. Dezember [1546]</t>
+          <t>Peter Kunz (Conzenus) / Bern an Heinrich Bullinger, 20. Oktober 1542</t>
         </is>
       </c>
       <c r="D117" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 77</t>
+          <t>Fussnote 28</t>
         </is>
       </c>
       <c r="E117" s="6" t="n"/>
@@ -2607,17 +2607,17 @@
     <row r="118">
       <c r="B118" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Scriptum est etiam idem nuper ex Venetiis, sicut in superioribus tibi scripsi literis,__77 quas interim te recepisse puto.</t>
+          <t>D. Eberardus a Rümlang, ut est iudicio perspicaci, ita fide inter me et te egit optima; nihil enim de me pollictus est tibi,__28 quod in literis meis non videas ex animo declaratum.</t>
         </is>
       </c>
       <c r="D118" s="7" t="inlineStr">
         <is>
-          <t>In Nr. 2712,34f, vom 10. Dezember. - Zur Angelegenheit s. Nr. 2725, Anm. 21.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E118" s="7" t="n"/>
@@ -2628,7 +2628,7 @@
     <row r="119">
       <c r="B119" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D119" s="8" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="120">
       <c r="B120" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D120" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. oben Nr. 1669, 2-36. 44-51; 1670, 17-25.</t>
         </is>
       </c>
       <c r="E120" s="7" t="n"/>
@@ -2676,7 +2676,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11755_2</t>
+          <t>11755_48</t>
         </is>
       </c>
       <c r="C122" s="6" t="inlineStr">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="D122" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 2</t>
+          <t>Fussnote 48</t>
         </is>
       </c>
       <c r="E122" s="6" t="n"/>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Exhibuerunt mihi nuper, charissime Bullingere, quidam fratres tuos in Mattheum commentarios obnixe rogantes, uti in 19. capite legerem tuam sententiam contra adsertores et defensores digamię;__2 sciebant enim te semper a me magnifieri.</t>
+          <t>Primum facis ex verbis Christi Matt. 19 [4-6. 8f] generalem canonem ad digamiam proculcandam__48.</t>
         </is>
       </c>
       <c r="D123" s="7" t="inlineStr">
@@ -2734,12 +2734,12 @@
     <row r="125">
       <c r="B125" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D125" s="7" t="inlineStr">
         <is>
-          <t>AaO, f. 179r.-v.: "Contra doctores polygamiae". -Als "digamia" bzw. "digamey" (eigentlich: Zweitehe) bezeichnet Lening evangelium auch Ehen mit mehr als zwei Frauen (vgl. dazu Bullingers Bemerkung unten Nr. 1723, 151).</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E125" s="7" t="n"/>
@@ -2750,12 +2750,12 @@
     <row r="126">
       <c r="B126" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D126" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>AaO (vgl. oben Anm. 1f), f. 179r., Z. 1.</t>
         </is>
       </c>
       <c r="E126" s="8" t="n"/>
@@ -2766,17 +2766,17 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>10963_7</t>
+          <t>12322_12</t>
         </is>
       </c>
       <c r="C127" s="6" t="inlineStr">
         <is>
-          <t>Johannes Zwick / [Konstanz] an [Heinrich Bullinger], [Leo Jud], [Konrad Pellikan (Kürschner)], [Theodor Bibliander (Buchmann)], 30. November 1536</t>
+          <t>Heinrich Bullinger / Zürich an Matthias Erb, 30. Oktober 1545</t>
         </is>
       </c>
       <c r="D127" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 7</t>
+          <t>Fussnote 12</t>
         </is>
       </c>
       <c r="E127" s="6" t="n"/>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Responsionem nostram etiam Sangallum misimus__7, item Lindavium.</t>
+          <t>Addam paulo post et praefationem in Ioannem De iustificatione hominis Christiani__12.</t>
         </is>
       </c>
       <c r="D128" s="7" t="inlineStr">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="D129" s="8" t="inlineStr">
         <is>
-          <t>Siehe Moeller, Zwick 254, Nr. 108; Vadian BW V 388f.</t>
+          <t>Bullingers Vorhaben, die Vorrede seines Johanneskommentars von 1543 (HBBibl I 153) gesondert herauszugeben, wurde erst 1548 (HBBibl 1157) verwirklicht.</t>
         </is>
       </c>
       <c r="E129" s="8" t="n"/>
@@ -2824,7 +2824,7 @@
     <row r="130">
       <c r="B130" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D130" s="7" t="inlineStr">
@@ -2840,7 +2840,7 @@
     <row r="131">
       <c r="B131" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D131" s="8" t="inlineStr">
@@ -2856,17 +2856,17 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>12331_4</t>
+          <t>11614_21</t>
         </is>
       </c>
       <c r="C132" s="6" t="inlineStr">
         <is>
-          <t>Heinrich Bullinger / Zürich an Ambrosius Blarer (Blaurer), 10. November 1545</t>
+          <t>Oswald Myconius (Geißhüsler) / Basel an Heinrich Bullinger, 22. September 1541</t>
         </is>
       </c>
       <c r="D132" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 4</t>
+          <t>Fussnote 21</t>
         </is>
       </c>
       <c r="E132" s="6" t="n"/>
@@ -2877,17 +2877,17 @@
     <row r="133">
       <c r="B133" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>N.__4 consultationem, pro qua ingentes ago gratias, remitto.</t>
+          <t>Et triste nuncium illud adde Zvinglium Argentinę defunctum, quamvis in pagum quendam__21 eum ab urbe seposuerint etc.</t>
         </is>
       </c>
       <c r="D133" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Nach Wasselnheim (Wasselonne, "Waßelen"; s. ebd.).</t>
         </is>
       </c>
       <c r="E133" s="7" t="n"/>
@@ -2914,7 +2914,7 @@
     <row r="135">
       <c r="B135" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D135" s="7" t="inlineStr">
@@ -2930,12 +2930,12 @@
     <row r="136">
       <c r="B136" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D136" s="8" t="inlineStr">
         <is>
-          <t>Damit ist der anonyme Verfasser des von Blarer zugeschickten Gutachtens gemeint.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E136" s="8" t="n"/>
@@ -2946,17 +2946,17 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>12182_5</t>
+          <t>10192_9</t>
         </is>
       </c>
       <c r="C137" s="6" t="inlineStr">
         <is>
-          <t>Heinrich Bullinger / Zürich an Eberhard von Rümlang, 14. April 1545</t>
+          <t>Berchtold Haller / [Bern] an Heinrich Bullinger, 14. Dezember 1532</t>
         </is>
       </c>
       <c r="D137" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 5</t>
+          <t>Fussnote 9</t>
         </is>
       </c>
       <c r="E137" s="6" t="n"/>
@@ -2967,12 +2967,12 @@
     <row r="138">
       <c r="B138" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Misimus enim amplissimo senatui Bernensi exemplum__5 una cum literis, ad quas nihil nobis responderunt, quamquam nullam responsionem postulaverimus.</t>
+          <t>Cęterum Salodorenses pii__9, qui in urbe sunt, extra urbem in pago quodam vicino verbum audiunt a fratre quodam, quem suis impensis fovent etsi modicissime.</t>
         </is>
       </c>
       <c r="D138" s="7" t="inlineStr">
@@ -2988,7 +2988,7 @@
     <row r="139">
       <c r="B139" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D139" s="8" t="inlineStr">
@@ -3004,7 +3004,7 @@
     <row r="140">
       <c r="B140" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D140" s="7" t="inlineStr">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D141" s="8" t="inlineStr">
         <is>
-          <t>Die deutsche Fassung, das "Warhaffte Bekanntnuß".</t>
+          <t>Zur Lage der Reformierten in Solothurn s. oben [Nr. 132] S. 237,3-19 und Haefliger 162-165.</t>
         </is>
       </c>
       <c r="E141" s="8" t="n"/>
@@ -3036,17 +3036,17 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11152_10</t>
+          <t>13003_2</t>
         </is>
       </c>
       <c r="C142" s="6" t="inlineStr">
         <is>
-          <t>Johannes Rhellikan (Müller aus Rellikon) / Bern an Heinrich Bullinger, Kaspar Megander (Großmann), 7. März 1538</t>
+          <t>Heinrich Bullinger / Zürich an Oswald Myconius (Geißhüsler), 16. Juli 1547</t>
         </is>
       </c>
       <c r="D142" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 10</t>
+          <t>Fussnote 2</t>
         </is>
       </c>
       <c r="E142" s="6" t="n"/>
@@ -3057,17 +3057,17 @@
     <row r="143">
       <c r="B143" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Quo fit, ut censeam hominem paulatim a lapsu erigendum et nobis illud Paulinum crebro occinendum: „Qui stat, videat, ne cadat“ et illud Senecae: „Quod uni alicui contingit, in simili casu omnibus contingere potest.“__10</t>
+          <t>Mulier illa tuas__2 mihi reddidit.</t>
         </is>
       </c>
       <c r="D143" s="7" t="inlineStr">
         <is>
-          <t>Die Quelle des Zitats konnte nicht nachgewiesen werden.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E143" s="7" t="n"/>
@@ -3078,12 +3078,12 @@
     <row r="144">
       <c r="B144" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D144" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Myconius' Brief vom 5. Juli (Nr. 2943).</t>
         </is>
       </c>
       <c r="E144" s="8" t="n"/>
@@ -3110,7 +3110,7 @@
     <row r="146">
       <c r="B146" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D146" s="8" t="inlineStr">
@@ -3126,17 +3126,17 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>12158_22</t>
+          <t>11456_29</t>
         </is>
       </c>
       <c r="C147" s="6" t="inlineStr">
         <is>
-          <t>Heinrich Bullinger / Zürich an Ambrosius Blarer (Blaurer), 16. März 1545</t>
+          <t>Rudolf Gwalther (Walter, Gualtherus, Walthart) d.Ä. / Marburg an Heinrich Bullinger, 4. August 1540</t>
         </is>
       </c>
       <c r="D147" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 22</t>
+          <t>Fussnote 29</t>
         </is>
       </c>
       <c r="E147" s="6" t="n"/>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Responsionem nostram Latinam fecit Gvaltherus, quae et ipsa impressa est__22.</t>
+          <t>Quid Saxonię dux__29 facturus sit, ignoratur, sed haud dubie vix inultum sinet.</t>
         </is>
       </c>
       <c r="D148" s="7" t="inlineStr">
@@ -3168,7 +3168,7 @@
     <row r="149">
       <c r="B149" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D149" s="8" t="inlineStr">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="D150" s="7" t="inlineStr">
         <is>
-          <t>Die "Orthodoxa Tigurinae eccleasiae confessio", die wohl zwischen dem 8. März (Datum des Nachworts des Übersetzers [Gwalther] an den Leser) und dem 12. März 1545 aus der Presse kam; s. oben Nr. 2061, Anm. 9.</t>
+          <t>Herzog Heinrich der Fromme, der Onkel der Landgräfin.</t>
         </is>
       </c>
       <c r="E150" s="7" t="n"/>
@@ -3200,7 +3200,7 @@
     <row r="151">
       <c r="B151" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D151" s="8" t="inlineStr">
@@ -3216,17 +3216,17 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12707_11</t>
+          <t>11503_9</t>
         </is>
       </c>
       <c r="C152" s="6" t="inlineStr">
         <is>
-          <t>Leonhard Serin (Soerinus) / Ulm an Heinrich Bullinger, 5. November 1546</t>
+          <t>Joachim Vadian (von Watt) / St. Gallen an Heinrich Bullinger, 8. Februar 1541</t>
         </is>
       </c>
       <c r="D152" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 11</t>
+          <t>Fussnote 9</t>
         </is>
       </c>
       <c r="E152" s="6" t="n"/>
@@ -3237,12 +3237,12 @@
     <row r="153">
       <c r="B153" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Nam, ut prius in manus ipsius quam meas errore latoris (quem ignoro, quisnam fuerit) pervenit, tam avide legit, ut mihi nonnisi perlecta folia__11 traderet optaretque Varnirium etiam excudere.</t>
+          <t>Mansum Alemanni fundum dixere cum villula.</t>
         </is>
       </c>
       <c r="D153" s="7" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="154">
       <c r="B154" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D154" s="8" t="inlineStr">
@@ -3274,12 +3274,12 @@
     <row r="155">
       <c r="B155" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D155" s="7" t="inlineStr">
         <is>
-          <t>Gemeint sind die einzelnen Lagen des noch nicht gebundenen Exemplars.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E155" s="7" t="n"/>
@@ -3290,12 +3290,12 @@
     <row r="156">
       <c r="B156" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D156" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Zum Begriff "mansus" vgl. unten Anm. 27.</t>
         </is>
       </c>
       <c r="E156" s="8" t="n"/>
@@ -3306,17 +3306,17 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11388_8</t>
+          <t>12258_28</t>
         </is>
       </c>
       <c r="C157" s="6" t="inlineStr">
         <is>
-          <t>[Johannes Zwick] / Konstanz an [Heinrich Bullinger], 1. Januar 1540</t>
+          <t>[Ambrosius Blarer (Blaurer)] / [Konstanz] an Heinrich Bullinger, 10. August 1545</t>
         </is>
       </c>
       <c r="D157" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 8</t>
+          <t>Fussnote 28</t>
         </is>
       </c>
       <c r="E157" s="6" t="n"/>
@@ -3327,17 +3327,17 @@
     <row r="158">
       <c r="B158" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Primum enim non videtur sine maximo offendiculo futurum, ut nostri iungantur vestris, neque satis causae esse ad defectionem ex eo, in quo etiamnum foedere sumus__8.</t>
+          <t>Nostri vero prorsus eas concessiones retinere voluerunt__28.</t>
         </is>
       </c>
       <c r="D158" s="7" t="inlineStr">
         <is>
-          <t>Konstanz gehörte seit 1531 dem Schmalkaldischen Bund an; vgl. Hermann Buck und Ekkehart Fabian, Konstanzer Reformationsgeschichte in ihren Grundzügen, I. Teil: 1519-1531, Tübingen 1965. - SKRG 25/26, S. 336-343.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E158" s="7" t="n"/>
@@ -3364,7 +3364,7 @@
     <row r="160">
       <c r="B160" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D160" s="7" t="inlineStr">
@@ -3380,12 +3380,12 @@
     <row r="161">
       <c r="B161" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D161" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>In ihrer Protestation vom 4. August 1545 erneuerten die Stände der Augsburger Konfession ihre Forderungen bezüglich Friede und Recht und lehnten das Konzil von Trient ab; s. RTA JR XVI/2 1669-1672, Nr. 342.</t>
         </is>
       </c>
       <c r="E161" s="8" t="n"/>
@@ -3396,17 +3396,17 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12071_2</t>
+          <t>10237_15</t>
         </is>
       </c>
       <c r="C162" s="6" t="inlineStr">
         <is>
-          <t>Johann Leopold (Lüpold) Frey / Biel an Heinrich Bullinger, 28. Oktober 1544</t>
+          <t>[Berchtold Haller] / [Bern] an Heinrich Bullinger, 31. März 1533</t>
         </is>
       </c>
       <c r="D162" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 2</t>
+          <t>Fussnote 15</t>
         </is>
       </c>
       <c r="E162" s="6" t="n"/>
@@ -3417,12 +3417,12 @@
     <row r="163">
       <c r="B163" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>In primis quae de rebus bellum attinentibus__2 ad me respondisti, non tam me quam alios quoque cordatos salutique nostrę consultum volentes fratres magnis affecerunt gaudiis.</t>
+          <t>Scis, quem velim__15.</t>
         </is>
       </c>
       <c r="D163" s="7" t="inlineStr">
@@ -3454,12 +3454,12 @@
     <row r="165">
       <c r="B165" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D165" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Wahrscheinlich Kaspar Megander, s. oben [Nr. 199] S. 84, Anm. 14; vgl. auch die Bemerkung von J. J. Simler zu dieser Stelle, Zürich ZB, Ms S 33, Nr. 74.</t>
         </is>
       </c>
       <c r="E165" s="7" t="n"/>
@@ -3470,12 +3470,12 @@
     <row r="166">
       <c r="B166" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D166" s="8" t="inlineStr">
         <is>
-          <t>Über den Krieg zwischen Karl V. und Franz I.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E166" s="8" t="n"/>
@@ -3486,7 +3486,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>11503_108</t>
+          <t>11503_19</t>
         </is>
       </c>
       <c r="C167" s="6" t="inlineStr">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="D167" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 108</t>
+          <t>Fussnote 19</t>
         </is>
       </c>
       <c r="E167" s="6" t="n"/>
@@ -3507,17 +3507,17 @@
     <row r="168">
       <c r="B168" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Sic quondam monachi nostri numeris et carmine ludebant, literis videlicet et musis, ut in ludo publico et celebri dediti, quum nostri hodie in otio saginati longe alias colant musas et nihil minus ament quam literas.__108</t>
+          <t>Quare et apochas dabant coloni, quibus de pac[to] et condictione, qua locatus erat ager, cavebatur, quas hodie vulg[o] literas reversi et lingua nostra reversbrief, locationem autem ip[sam] erblehen__19 vocamus.</t>
         </is>
       </c>
       <c r="D168" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vererbliches Lehen, vgl. DRW III 95.</t>
         </is>
       </c>
       <c r="E168" s="7" t="n"/>
@@ -3544,12 +3544,12 @@
     <row r="170">
       <c r="B170" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D170" s="7" t="inlineStr">
         <is>
-          <t>Zu Vadians negativer Beurteilung der Entwicklung der monastischen Bildung und Gelehrsamkeit vgl. u. a. dessen "Farrago" (Goldast, aaO, Bd. III, S. 2f).</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E170" s="7" t="n"/>
@@ -3576,17 +3576,17 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12818_8</t>
+          <t>10614_5</t>
         </is>
       </c>
       <c r="C172" s="6" t="inlineStr">
         <is>
-          <t>Johannes Haller d.J. / Augsburg an Heinrich Bullinger, 25. Januar 1547</t>
+          <t>Berchtold Haller / [Bern] an Heinrich Bullinger, 22. April 1535</t>
         </is>
       </c>
       <c r="D172" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 8</t>
+          <t>Fussnote 5</t>
         </is>
       </c>
       <c r="E172" s="6" t="n"/>
@@ -3597,12 +3597,12 @@
     <row r="173">
       <c r="B173" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Hoc effecerunt nebulones illi monopolae__8, publicani, etc., qui inhonestam potius volunt habere pacem quam periculosam libertatem, quam crucem tollere velint Christi.</t>
+          <t>Nuncius est tutissimus, unus a Madiis, Jacobi a Madiis frater__5, qui reducet ab Enocho mortuo duos germanos.</t>
         </is>
       </c>
       <c r="D173" s="7" t="inlineStr">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="D174" s="8" t="inlineStr">
         <is>
-          <t>Kauf- und Handelsleute mit einem Monopol; vgl. Kirsch 1811.</t>
+          <t>Welcher Bruder von Jakob May gemeint ist, konnte nicht festgestellt werden.</t>
         </is>
       </c>
       <c r="E174" s="8" t="n"/>
@@ -3634,7 +3634,7 @@
     <row r="175">
       <c r="B175" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D175" s="7" t="inlineStr">
@@ -3650,7 +3650,7 @@
     <row r="176">
       <c r="B176" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D176" s="8" t="inlineStr">
@@ -3666,17 +3666,17 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10389_32</t>
+          <t>10506_31</t>
         </is>
       </c>
       <c r="C177" s="6" t="inlineStr">
         <is>
-          <t>Berchtold Haller / [Bern] an Heinrich Bullinger, 18. April 1534</t>
+          <t>Martin Bucer / Tübingen an Heinrich Bullinger, [1. November 1534]</t>
         </is>
       </c>
       <c r="D177" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 32</t>
+          <t>Fussnote 31</t>
         </is>
       </c>
       <c r="E177" s="6" t="n"/>
@@ -3687,12 +3687,12 @@
     <row r="178">
       <c r="B178" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Megander inprimi vult sua in Ephesios__32.</t>
+          <t>De quo quid scripseris, tu nosti, et consonat ei testimonio confessio vestra missa Blaurero__31.</t>
         </is>
       </c>
       <c r="D178" s="7" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="179">
       <c r="B179" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D179" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die schon in Anm. 2 erwähnte Nr. 463.</t>
         </is>
       </c>
       <c r="E179" s="8" t="n"/>
@@ -3724,7 +3724,7 @@
     <row r="180">
       <c r="B180" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D180" s="7" t="inlineStr">
@@ -3740,12 +3740,12 @@
     <row r="181">
       <c r="B181" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D181" s="8" t="inlineStr">
         <is>
-          <t>«Gasparis Megandri Tigurini, in epistolam Pauli ad Ephesios commentarius: Vnà cum Ioannis Rhellicani epistola monitoria» erschien im August 1534 bei Heinrich Petri in Basel. Vgl. auch HBBW III [Nr. 199] 85f, 69-74. 149, 31. 274, 36f.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E181" s="8" t="n"/>
@@ -3756,17 +3756,17 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11888_10</t>
+          <t>11764_9</t>
         </is>
       </c>
       <c r="C182" s="6" t="inlineStr">
         <is>
-          <t>Heinrich Bullinger / Zürich an Eberhard von Rümlang, 31. Januar 1544</t>
+          <t>Oswald Pergener / Zittau an Heinrich Bullinger, 8. Februar 1543</t>
         </is>
       </c>
       <c r="D182" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 10</t>
+          <t>Fussnote 9</t>
         </is>
       </c>
       <c r="E182" s="6" t="n"/>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Esse illis disputata et certa religionis capita, quibus adhaerere velle et in ipsis permanere testentur legati, qui Badenam__10 veniant.</t>
+          <t>Docet nos quoque d. Chuonradus Pellicanus in septem suis tomis super libros Biblię,__9 et in aliis idem faciunt sanctissimi martires et viri Hul[drichus] Tzving[lius], Ioh[annes] Oecolamp[adius].</t>
         </is>
       </c>
       <c r="D183" s="7" t="inlineStr">
@@ -3798,7 +3798,7 @@
     <row r="184">
       <c r="B184" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D184" s="8" t="inlineStr">
@@ -3814,12 +3814,12 @@
     <row r="185">
       <c r="B185" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D185" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Zu Pellikans Kommentarwerk s. HBBW XII [Nr. 1646], S. 148f, Anm. 57.</t>
         </is>
       </c>
       <c r="E185" s="7" t="n"/>
@@ -3830,12 +3830,12 @@
     <row r="186">
       <c r="B186" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D186" s="8" t="inlineStr">
         <is>
-          <t>zu den eidgenössischen Tagsatzungen.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E186" s="8" t="n"/>
@@ -3846,17 +3846,17 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10633_4</t>
+          <t>12938_24</t>
         </is>
       </c>
       <c r="C187" s="6" t="inlineStr">
         <is>
-          <t>Florian Chinlius / Malans an Heinrich Bullinger, 22. Juni 1535</t>
+          <t>Theobald Thamer / Marburg an Heinrich Bullinger, 27. April 1547</t>
         </is>
       </c>
       <c r="D187" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 4</t>
+          <t>Fussnote 24</t>
         </is>
       </c>
       <c r="E187" s="6" t="n"/>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Humanissime frater, nota tibi illa iuris regula omne promissum cadere in debitum__4.</t>
+          <t>Commendo tibi hosce duos adulescentes__24, quamquam nihil dubitem eos sicut omnes studiosos et religione et naturali vita tibi commendatos.</t>
         </is>
       </c>
       <c r="D188" s="7" t="inlineStr">
@@ -3888,7 +3888,7 @@
     <row r="189">
       <c r="B189" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D189" s="8" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="D190" s="7" t="inlineStr">
         <is>
-          <t>Vgl. Wander V 649.</t>
+          <t>Johannes und Justus Vulteius.</t>
         </is>
       </c>
       <c r="E190" s="7" t="n"/>
@@ -3920,7 +3920,7 @@
     <row r="191">
       <c r="B191" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D191" s="8" t="inlineStr">
@@ -3936,17 +3936,17 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>10348_39</t>
+          <t>11537_34</t>
         </is>
       </c>
       <c r="C192" s="6" t="inlineStr">
         <is>
-          <t>Ambrosius Blarer (Blaurer) / [Konstanz] an Heinrich Bullinger, 20. Januar 1534</t>
+          <t>Johannes Wolf / Frankfurt am Main an Heinrich Bullinger, 10. April 1541</t>
         </is>
       </c>
       <c r="D192" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 39</t>
+          <t>Fussnote 34</t>
         </is>
       </c>
       <c r="E192" s="6" t="n"/>
@@ -3957,12 +3957,12 @@
     <row r="193">
       <c r="B193" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Sic, sic, mi Bullingere, vix adhuc in lucem ędito Christo apud Gallos Herodes__39 insidiatur, ut perdat.</t>
+          <t>Salutabis, obsecro, familiam tuam, in primis coniugem__34 tuam et matrem, quas ego mihi quam optime velle hactenus semper sum expertus.</t>
         </is>
       </c>
       <c r="D193" s="7" t="inlineStr">
@@ -3978,12 +3978,12 @@
     <row r="194">
       <c r="B194" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D194" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Anna, geb. Adlischwyler.</t>
         </is>
       </c>
       <c r="E194" s="8" t="n"/>
@@ -3994,7 +3994,7 @@
     <row r="195">
       <c r="B195" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model1</t>
         </is>
       </c>
       <c r="D195" s="7" t="inlineStr">
@@ -4010,12 +4010,12 @@
     <row r="196">
       <c r="B196" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D196" s="8" t="inlineStr">
         <is>
-          <t>Gemeint ist Franz I.</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E196" s="8" t="n"/>
@@ -4026,17 +4026,17 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>10560_13</t>
+          <t>11537_20</t>
         </is>
       </c>
       <c r="C197" s="6" t="inlineStr">
         <is>
-          <t>Berchtold Haller / [Bern] an Heinrich Bullinger, 9. Februar 1535</t>
+          <t>Johannes Wolf / Frankfurt am Main an Heinrich Bullinger, 10. April 1541</t>
         </is>
       </c>
       <c r="D197" s="6" t="inlineStr">
         <is>
-          <t>Fussnote 13</t>
+          <t>Fussnote 20</t>
         </is>
       </c>
       <c r="E197" s="6" t="n"/>
@@ -4047,17 +4047,17 @@
     <row r="198">
       <c r="B198" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Nam ad Arouw__13 ego nec pedes nec eques venire valeo.</t>
+          <t>Alteram__20 vidi gravidam, et mox quoque parituram aut iamiam peperisse arbitror.</t>
         </is>
       </c>
       <c r="D198" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Landgräfin Christine von Hessen.</t>
         </is>
       </c>
       <c r="E198" s="7" t="n"/>
@@ -4068,12 +4068,12 @@
     <row r="199">
       <c r="B199" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>model2</t>
         </is>
       </c>
       <c r="D199" s="8" t="inlineStr">
         <is>
-          <t>Aarau (Kt. Aargau).</t>
+          <t>Lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E199" s="8" t="n"/>
@@ -4100,7 +4100,7 @@
     <row r="201">
       <c r="B201" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D201" s="8" t="inlineStr">

</xml_diff>

<commit_message>
add model responses to human eval sheet, starting with a run of GPT-4
</commit_message>
<xml_diff>
--- a/evaluate/human_eval/evaluation_form_v1.xlsx
+++ b/evaluate/human_eval/evaluation_form_v1.xlsx
@@ -537,7 +537,7 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D3" s="7" t="inlineStr">
         <is>
-          <t>Vgl. 1Kor 7, 25.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E3" s="7" t="n"/>
@@ -558,12 +558,12 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1Kor 7, 25.</t>
         </is>
       </c>
       <c r="E4" s="8" t="n"/>
@@ -574,12 +574,12 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E5" s="7" t="n"/>
@@ -590,12 +590,12 @@
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der Ausdruck "ad Kalendas Graecas" stammt aus der Antike und bedeutet etwa "an einem niemals eintretenden Zeitpunkt". Er wurde von Kaiser Augustus geprägt, um Überschuldete zu beruhigen, da es im alten Griechenland keine Kalenden, d.h. keinen ersten Tag im Monat, gab. Lening spielt hier darauf an, dass Bullinger erst dann das Unmögliche beweisen kann, wenn er seine eigene Lehre widerspricht und den heilsamen Aspekt der göttlichen Dispensation ignoriert.</t>
         </is>
       </c>
       <c r="E6" s="8" t="n"/>
@@ -627,7 +627,7 @@
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -637,7 +637,7 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1 Kor 7,2. 28. 36.</t>
         </is>
       </c>
       <c r="E8" s="7" t="n"/>
@@ -648,12 +648,12 @@
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E9" s="8" t="n"/>
@@ -664,12 +664,12 @@
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E10" s="7" t="n"/>
@@ -680,12 +680,12 @@
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>Vgl. 1 Kor 7,2. 28. 36.</t>
+          <t>Bullinger verteidigt hier die Ehe als einen göttlich eingesetzten Stand, der nicht per se sündhaft ist. Dies verweist auf die reformatorische Ablehnung der klösterlichen Gelübde und unterstreicht die Bedeutung der Ehe als gleichwertige und tugendhafte Lebensform im Gegensatz zum klösterlichen Leben.</t>
         </is>
       </c>
       <c r="E11" s="8" t="n"/>
@@ -717,7 +717,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="D13" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Siehe oben Anm. 53.</t>
         </is>
       </c>
       <c r="E13" s="7" t="n"/>
@@ -738,12 +738,12 @@
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>Siehe oben Anm. 53.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E14" s="8" t="n"/>
@@ -754,12 +754,12 @@
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D15" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>„Vortgetruckt“ in diesem Kontext bedeutet einen militärischen Vorstoß oder Angriff. Der Begriff wurde häufig verwendet, um den Vormarsch oder das Fortschreiten von Truppen in Richtung des Feindes zu beschreiben. Am 2. September 1546 wurde ein Angriff auf die feindlichen Positionen ausgeführt, der als erfolgreich beschrieben wird, indem er erheblichen Schaden verursachte.</t>
         </is>
       </c>
       <c r="E15" s="7" t="n"/>
@@ -770,12 +770,12 @@
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E16" s="8" t="n"/>
@@ -807,7 +807,7 @@
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="D18" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E18" s="7" t="n"/>
@@ -844,12 +844,12 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D20" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Das erwähnte Schreiben könnte sich auf Korrespondenz im Kontext des Schmalkaldischen Krieges beziehen, der 1546 begann und in dem die protestantischen Fürsten gegen Kaiser Karl V. und seine katholischen Verbündeten kämpften. Es ist möglich, dass das Schreiben militärische oder diplomatische Angelegenheiten betraf und von hoher strategischer Bedeutung für die protestantischen Bündnispartner, zu denen Ambrosius Blarer und Heinrich Bullinger gehörten, war.</t>
         </is>
       </c>
       <c r="E20" s="7" t="n"/>
@@ -860,12 +860,12 @@
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E21" s="8" t="n"/>
@@ -897,7 +897,7 @@
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="D23" s="7" t="inlineStr">
         <is>
-          <t>König Ferdinand und Christoph von Württemberg einigten sich nicht, vgl. unten Z. 77-81 und Wille 120-130. 137f. 141-144.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E23" s="7" t="n"/>
@@ -918,12 +918,12 @@
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>König Ferdinand und Christoph von Württemberg einigten sich nicht, vgl. unten Z. 77-81 und Wille 120-130. 137f. 141-144.</t>
         </is>
       </c>
       <c r="E24" s="8" t="n"/>
@@ -934,12 +934,12 @@
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D25" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E25" s="7" t="n"/>
@@ -950,12 +950,12 @@
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die Verhandlungen zwischen der königlichen Majestät und Herzog Christoph von Württemberg bezogen sich auf die Rückerlangung seines Herzogtums, das sein Vater im Jahre 1519 verloren hatte. Die Reichspolitik war durch die Absichten des Kaisers Karl V. geprägt, der die Unterstützung der deutschen Fürsten benötigte, um seine Macht im Reich zu sichern.</t>
         </is>
       </c>
       <c r="E26" s="8" t="n"/>
@@ -987,7 +987,7 @@
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="D28" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E28" s="7" t="n"/>
@@ -1008,12 +1008,12 @@
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der "gmain oder grossen radt" (gemeiner oder großer Rat) bezeichnet die Stadtversammlung oder den Stadtrat, wie es in vielen Reichsstädten des Heiligen Römischen Reiches üblich war. Diese Versammlungen waren zentrale Organe in der städtischen Selbstverwaltung und traten häufig zusammen, um wichtige politische, religiöse oder wirtschaftliche Entscheidungen zu verhandeln. Die Erwähnung einer solchen Ratsversammlung in Augsburg im Jahr 1534 könnte im Kontext der Reformation stehen, als viele Städte in konfessionellen Fragen Entscheidungen trafen.</t>
         </is>
       </c>
       <c r="E29" s="8" t="n"/>
@@ -1040,12 +1040,12 @@
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E31" s="8" t="n"/>
@@ -1077,7 +1077,7 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D33" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E33" s="7" t="n"/>
@@ -1098,12 +1098,12 @@
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die Redewendung "Hand zu wordt" bedeutet, dass Taten den Worten folgen müssen oder dass Versprechen in die Tat umgesetzt werden sollen. In diesem Kontext betont Johannes Haab möglicherweise die Notwendigkeit, entschlossen zu handeln, anstatt nur darüber zu sprechen, in eine militärische Auseinandersetzung einzutreten.</t>
         </is>
       </c>
       <c r="E34" s="8" t="n"/>
@@ -1114,12 +1114,12 @@
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D35" s="7" t="inlineStr">
         <is>
-          <t>Hand zu wordt: Sie geben vor.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E35" s="7" t="n"/>
@@ -1130,12 +1130,12 @@
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D36" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Hand zu wordt: Sie geben vor.</t>
         </is>
       </c>
       <c r="E36" s="8" t="n"/>
@@ -1167,7 +1167,7 @@
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D38" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>HBBibl I 54; vgl. oben Anm. 39.</t>
         </is>
       </c>
       <c r="E38" s="7" t="n"/>
@@ -1188,12 +1188,12 @@
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D39" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E39" s="8" t="n"/>
@@ -1204,12 +1204,12 @@
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D40" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Heinrich Bullingers Werk „De unico et aeterno Testamento Dei“ wurde 1534 veröffentlicht. In diesem Werk verteidigt Bullinger die Einheit und Kontinuität des göttlichen Testaments und behandelt Aspekte der Theologie, die auch im Diskurs gegen die Täufer von Bedeutung waren.</t>
         </is>
       </c>
       <c r="E40" s="7" t="n"/>
@@ -1220,12 +1220,12 @@
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D41" s="8" t="inlineStr">
         <is>
-          <t>HBBibl I 54; vgl. oben Anm. 39.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E41" s="8" t="n"/>
@@ -1257,7 +1257,7 @@
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E43" s="7" t="n"/>
@@ -1278,12 +1278,12 @@
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D44" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. Lang, aaO, f. Biij,r.-v.; und [Enzinas], aaO, S. 137-142, wo das Ganze noch ausführlicher geschildert wird.</t>
         </is>
       </c>
       <c r="E44" s="8" t="n"/>
@@ -1294,12 +1294,12 @@
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D45" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E45" s="7" t="n"/>
@@ -1310,12 +1310,12 @@
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D46" s="8" t="inlineStr">
         <is>
-          <t>Vgl. Lang, aaO, f. Biij,r.-v.; und [Enzinas], aaO, S. 137-142, wo das Ganze noch ausführlicher geschildert wird.</t>
+          <t>Der Mord an Johannes Diacius, einem Anhänger der Reformation, durch seinen eigenen Bruder Alphonsus Diazius, einem katholischen Richter, ist ein historisches Ereignis, das die konfessionellen Spannungen der Zeit widerspiegelt. Diese Tat geschah 1546 in Augsburg, während einer Epoche, in der reformatorisches und katholisches Gedankengut häufig zu offenen Konflikten führte. Die Schilderung des Vorfalls in diesem Brief zeigt die Dramatik und die Gefährdung derjenigen, die sich zur Reformation bekannten. Siehe dazu auch die Anmerkungen von Heinrich Bullinger in seinen Aufzeichnungen bezüglich der Konsequenzen für die beteiligten Personen, insbesondere die Maßnahmen gegen Alphonsus nach seiner Festnahme in Innsbruck.</t>
         </is>
       </c>
       <c r="E46" s="8" t="n"/>
@@ -1368,12 +1368,12 @@
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D49" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E49" s="8" t="n"/>
@@ -1384,12 +1384,12 @@
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D50" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E50" s="7" t="n"/>
@@ -1400,12 +1400,12 @@
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D51" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Rornfels (möglicherweise ein Missverständnis oder eine Schreibvariante für die Ortschaft oder Region Rornfels/Rorhbach, die nicht eindeutig identifiziert werden kann).</t>
         </is>
       </c>
       <c r="E51" s="8" t="n"/>
@@ -1437,7 +1437,7 @@
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D53" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E53" s="7" t="n"/>
@@ -1458,12 +1458,12 @@
     <row r="54">
       <c r="B54" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D54" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der "Brunschwigische Krieg" bezieht sich auf den Konflikt um das Herzogtum Braunschweig-Lüneburg, bekannt als der "Hildesheimer Stiftsfehde", ein Konflikt zwischen dem Fürstbistum Hildesheim und den Welfischen Fürsten, der sich von 1519 bis 1523 erstreckte. In diesem Kontext könnte es sich jedoch auch um den Einfluss oder die nähere Bedrohung durch die Fehde oder ihre politischen Folgen handeln, die in späteren Jahren relevant waren.</t>
         </is>
       </c>
       <c r="E54" s="8" t="n"/>
@@ -1474,12 +1474,12 @@
     <row r="55">
       <c r="B55" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D55" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Siehe dazu Nr. 2452, Anm. 2.</t>
         </is>
       </c>
       <c r="E55" s="7" t="n"/>
@@ -1490,12 +1490,12 @@
     <row r="56">
       <c r="B56" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D56" s="8" t="inlineStr">
         <is>
-          <t>Siehe dazu Nr. 2452, Anm. 2.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E56" s="8" t="n"/>
@@ -1527,7 +1527,7 @@
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="D58" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E58" s="7" t="n"/>
@@ -1548,12 +1548,12 @@
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D59" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der eingefügte Zettel enthält zusätzliche Informationen oder spezifische Details, die nicht im Haupttext des Briefes enthalten sind. Solche Einlagen waren üblich, um vertrauliche oder detaillierte Anweisungen zu geben. Es war nicht unüblich, dass vertrauliche Mitteilungen oder wichtige Informationen in separaten Notizen übermittelt wurden, die dann später zerstört oder anderweitig behandelt wurden, um die Vertraulichkeit zu wahren.</t>
         </is>
       </c>
       <c r="E59" s="8" t="n"/>
@@ -1564,12 +1564,12 @@
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D60" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vermutlich waren es diese beiden Dokumente, die Blarer am 26. Dezember zurückverlangte; s. oben .</t>
         </is>
       </c>
       <c r="E60" s="7" t="n"/>
@@ -1580,12 +1580,12 @@
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D61" s="8" t="inlineStr">
         <is>
-          <t>Vermutlich waren es diese beiden Dokumente, die Blarer am 26. Dezember zurückverlangte; s. oben .</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E61" s="8" t="n"/>
@@ -1617,7 +1617,7 @@
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D63" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E63" s="7" t="n"/>
@@ -1638,12 +1638,12 @@
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D64" s="8" t="inlineStr">
         <is>
-          <t>Seit 1529 bzw. 1530 galt in Bern ein strenges Pensionen- und Reislaufverbot (SSRQ Bern I 11 362-368, vgl. Z XI 480, Anm. 4).</t>
+          <t>Die "Ordnung der reisglöffen" bezieht sich auf die Disposition oder den Marschbefehl der Berner Truppen, welcher offensichtlich bestimmte Voraussetzungen für ihre Rückkehr oder den weiteren Verlauf ihrer Mission forderte. Es könnte sich um logistische, taktische oder diplomatische Anweisungen gehandelt haben.</t>
         </is>
       </c>
       <c r="E64" s="8" t="n"/>
@@ -1654,12 +1654,12 @@
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D65" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E65" s="7" t="n"/>
@@ -1670,12 +1670,12 @@
     <row r="66">
       <c r="B66" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D66" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Seit 1529 bzw. 1530 galt in Bern ein strenges Pensionen- und Reislaufverbot (SSRQ Bern I 11 362-368, vgl. Z XI 480, Anm. 4).</t>
         </is>
       </c>
       <c r="E66" s="8" t="n"/>
@@ -1707,7 +1707,7 @@
     <row r="68">
       <c r="B68" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="D68" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E68" s="7" t="n"/>
@@ -1728,12 +1728,12 @@
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D69" s="8" t="inlineStr">
         <is>
-          <t>Die katholischen Orte, die mit Zürich den Thurgau verwalteten.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E69" s="8" t="n"/>
@@ -1744,12 +1744,12 @@
     <row r="70">
       <c r="B70" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D70" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die katholischen Orte, die mit Zürich den Thurgau verwalteten.</t>
         </is>
       </c>
       <c r="E70" s="7" t="n"/>
@@ -1760,12 +1760,12 @@
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D71" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die Erwähnung der "anderen Eidgenossen" bezieht sich auf die politischen und konfessionellen Beziehungen zwischen den verschiedenen Kantonen der Eidgenossenschaft. Zur Zeit des Schreibens waren die religiösen Spannungen hoch, insbesondere zwischen den reformierten und katholischen Kantonen. Diese Dynamik beeinflusste auch rechtliche Fragen und Entscheidungen, wie etwa die oben diskutierte Eheschließung und das Paar im Turgau.</t>
         </is>
       </c>
       <c r="E71" s="8" t="n"/>
@@ -1797,7 +1797,7 @@
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D73" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E73" s="7" t="n"/>
@@ -1818,12 +1818,12 @@
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D74" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E74" s="8" t="n"/>
@@ -1834,12 +1834,12 @@
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D75" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Zu dieser Route des niederländischen Heeres unter Maximilian von Egmont, Graf von Büren, auf dem Weg zum kaiserlichen Lager s. HBBW XVII 415, Anm. 43.</t>
         </is>
       </c>
       <c r="E75" s="7" t="n"/>
@@ -1850,12 +1850,12 @@
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D76" s="8" t="inlineStr">
         <is>
-          <t>Zu dieser Route des niederländischen Heeres unter Maximilian von Egmont, Graf von Büren, auf dem Weg zum kaiserlichen Lager s. HBBW XVII 415, Anm. 43.</t>
+          <t>Dieser Abschnitt ist Teil der strategischen Überlegungen im Zusammenhang mit den Auseinandersetzungen des Schmalkaldischen Krieges (1546–1547), bei dem der Kaiser versuchte, seine Kontrolle über die protestantischen Fürsten im Heiligen Römischen Reich auszudehnen. Der von Johannes Gast erwähnte „Weg, den die Niderlender heruff synt zogen“, könnte auf die Bewegungen der kaiserlichen Truppen hinweisen, die aus den Niederlanden kommend, den protestantischen Gebieten Deutschlands entgegenzogen, um diese zu unterwerfen.</t>
         </is>
       </c>
       <c r="E76" s="8" t="n"/>
@@ -1887,7 +1887,7 @@
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="D78" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E78" s="7" t="n"/>
@@ -1908,12 +1908,12 @@
     <row r="79">
       <c r="B79" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D79" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E79" s="8" t="n"/>
@@ -1924,12 +1924,12 @@
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D80" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>"In dieser diplomatischen Korrespondenz kann man beobachten, dass die Beteiligten bestrebt sind, konfliktträchtige Themen zu vermeiden, bis sie die gewünschten Zugeständnisse in den für die kaiserlichen Majestäten dringlichsten Angelegenheiten erreicht haben."</t>
         </is>
       </c>
       <c r="E80" s="7" t="n"/>
@@ -1998,12 +1998,12 @@
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D84" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E84" s="8" t="n"/>
@@ -2014,12 +2014,12 @@
     <row r="85">
       <c r="B85" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D85" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E85" s="7" t="n"/>
@@ -2030,12 +2030,12 @@
     <row r="86">
       <c r="B86" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D86" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Ein "nachpurlichs mittlyden gebärdet" bezieht sich auf ein nachbarliches Mitleid, das die Ratsherren von Lindau gegenüber den Empfängern des Mandats kundtaten. Diese Formulierung zeigt, dass die Ratsherren bedauerten, ein Mandat überbracht zu haben, wahrscheinlich im Rahmen von politischen Maßnahmen oder Konflikten, die nicht in ihrem Einflussbereich lagen und dennoch umgesetzt werden mussten.</t>
         </is>
       </c>
       <c r="E86" s="8" t="n"/>
@@ -2067,7 +2067,7 @@
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="D88" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E88" s="7" t="n"/>
@@ -2088,12 +2088,12 @@
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D89" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>"Daniden" scheint im Kontext des Briefes das Synonym für eine Begräbnisstätte zu sein, welches sich möglicherweise auf eine lokale oder altsprachliche Eigenheit bezieht. Ein "Schwäher" (Schwiegervater) hätte demnach eine von der reformierten Ordnung abweichende Bestattung arrangiert, wobei Elemente wie Kerzen, Weihwasser und Gesang verwendet werden. Solche Rituale waren aus reformatorischer Sicht umstritten. Beachten Sie, dass solche Begräbnisse Teil der umfänglicheren Konfessionskonflikte der Zeit waren, in denen die alten katholischen Bräuche stark in Frage gestellt wurden.</t>
         </is>
       </c>
       <c r="E89" s="8" t="n"/>
@@ -2120,12 +2120,12 @@
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D91" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E91" s="8" t="n"/>
@@ -2157,7 +2157,7 @@
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D93" s="7" t="inlineStr">
         <is>
-          <t>(Er) solle (sie).</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E93" s="7" t="n"/>
@@ -2178,12 +2178,12 @@
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D94" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Das Wort "Soͤlly" bezieht sich vermutlich auf eine Verantwortungsübernahme oder eine Verpflichtung, genauer genommen könnte es "sollen" bedeuten, im Sinne von "diese haben für Euch gegeben" oder "sie sollen es für Euch geben".</t>
         </is>
       </c>
       <c r="E94" s="8" t="n"/>
@@ -2194,12 +2194,12 @@
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D95" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E95" s="7" t="n"/>
@@ -2210,12 +2210,12 @@
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D96" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>(Er) solle (sie).</t>
         </is>
       </c>
       <c r="E96" s="8" t="n"/>
@@ -2247,7 +2247,7 @@
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="D98" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E98" s="7" t="n"/>
@@ -2268,12 +2268,12 @@
     <row r="99">
       <c r="B99" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D99" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>vor 14 Tagen.</t>
         </is>
       </c>
       <c r="E99" s="8" t="n"/>
@@ -2284,12 +2284,12 @@
     <row r="100">
       <c r="B100" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D100" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>„Mittwoch nach Laetare“ bezieht sich auf den Mittwoch nach dem vierten Sonntag der Fastenzeit, der als Laetare-Sonntag bekannt ist. Im Jahr 1534 fiel dieser auf den 11. März, was die Datierung der Versammlung am Mittwoch, den 25. Februar 1534, ergibt.</t>
         </is>
       </c>
       <c r="E100" s="7" t="n"/>
@@ -2300,12 +2300,12 @@
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D101" s="8" t="inlineStr">
         <is>
-          <t>vor 14 Tagen.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E101" s="8" t="n"/>
@@ -2337,7 +2337,7 @@
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D103" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E103" s="7" t="n"/>
@@ -2358,12 +2358,12 @@
     <row r="104">
       <c r="B104" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D104" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E104" s="8" t="n"/>
@@ -2390,12 +2390,12 @@
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D106" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der Ausdruck "carnis internitionem spiritus alimentum esse" im Brief von Gervasius Schuler an Heinrich Bullinger spiegelt eine gängige theologische Sichtweise der Reformationszeit wider, die aus der paulinischen Theologie der Kreuzigung des Fleisches (vgl. Galater 5,24) abgeleitet ist und im Kontext der asketischen Praxis interpretiert wird. Das Töten des Fleisches wird als Nahrung für den Geist angesehen, was den Wert des Leidens im Streben nach spiritueller Erbauung und Nähe zu Gott betont.</t>
         </is>
       </c>
       <c r="E106" s="8" t="n"/>
@@ -2427,7 +2427,7 @@
     <row r="108">
       <c r="B108" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="D108" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E108" s="7" t="n"/>
@@ -2464,12 +2464,12 @@
     <row r="110">
       <c r="B110" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D110" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die Redewendung "abundare in sensu suo" stammt aus der Vulgata, dem lateinischen Text der Bibel, und bedeutet wörtlich "in seiner eigenen Meinung reichlich sein". Im übertragenen Sinne wird es als Aufforderung verstanden, bei der eigenen Meinung zu bleiben, ohne sich von äußeren Einflüssen oder Widerspruch beeindrucken zu lassen. Diese Redewendung drückt eine gewisse Toleranz gegenüber unterschiedlichen Ansichten aus und findet sich oft in theologischen Diskussionen der Reformationszeit.</t>
         </is>
       </c>
       <c r="E110" s="7" t="n"/>
@@ -2480,12 +2480,12 @@
     <row r="111">
       <c r="B111" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D111" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E111" s="8" t="n"/>
@@ -2517,7 +2517,7 @@
     <row r="113">
       <c r="B113" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="D113" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>In diesem Abschnitt des Briefes betont Bullinger seine Unvoreingenommenheit und die Bereitschaft zur Zusammenarbeit. Das Wort "praeiuditio" steht hier für Vorurteil oder Voreingenommenheit. Er drückt aus, dass seine Überlegungen und Absichten frei von persönlichen Vorurteilen sind. Angesichts ihrer gemeinsamen Anstrengungen unterstreicht er die Hoffnung auf das Beste, insbesondere im Hinblick auf die Zusammenarbeit mit Ambrosius Blarer und Simon Grynaeus. Diese Passage soll Vertrauen und Einigkeit in der theologischen Diskussion stärken.</t>
         </is>
       </c>
       <c r="E113" s="7" t="n"/>
@@ -2538,12 +2538,12 @@
     <row r="114">
       <c r="B114" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D114" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E114" s="8" t="n"/>
@@ -2554,12 +2554,12 @@
     <row r="115">
       <c r="B115" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D115" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E115" s="7" t="n"/>
@@ -2607,7 +2607,7 @@
     <row r="118">
       <c r="B118" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="D118" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E118" s="7" t="n"/>
@@ -2628,12 +2628,12 @@
     <row r="119">
       <c r="B119" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D119" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Eberardus a Rümlang, ein Zeitgenosse und Vermittler im Austausch zwischen Kunz und Bullinger, ist hier als vertrauenswürdiger Zeuge und Mittler dargestellt. Die Unterstützung und die Vertrauenswürdigkeit seiner Aussagen sollen jegliche Zweifel an Kunz' Absichten ausräumen.</t>
         </is>
       </c>
       <c r="E119" s="8" t="n"/>
@@ -2644,12 +2644,12 @@
     <row r="120">
       <c r="B120" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D120" s="7" t="inlineStr">
         <is>
-          <t>Vgl. oben Nr. 1669, 2-36. 44-51; 1670, 17-25.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E120" s="7" t="n"/>
@@ -2660,12 +2660,12 @@
     <row r="121">
       <c r="B121" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D121" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. oben Nr. 1669, 2-36. 44-51; 1670, 17-25.</t>
         </is>
       </c>
       <c r="E121" s="8" t="n"/>
@@ -2697,7 +2697,7 @@
     <row r="123">
       <c r="B123" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="D123" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E123" s="7" t="n"/>
@@ -2718,12 +2718,12 @@
     <row r="124">
       <c r="B124" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D124" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>AaO (vgl. oben Anm. 1f), f. 179r., Z. 1.</t>
         </is>
       </c>
       <c r="E124" s="8" t="n"/>
@@ -2734,12 +2734,12 @@
     <row r="125">
       <c r="B125" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D125" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E125" s="7" t="n"/>
@@ -2750,12 +2750,12 @@
     <row r="126">
       <c r="B126" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D126" s="8" t="inlineStr">
         <is>
-          <t>AaO (vgl. oben Anm. 1f), f. 179r., Z. 1.</t>
+          <t>Heinrich Bullinger hatte in seinem Kommentar zu Matthäus 19, 4-6 dargelegt, dass die Ehe als unauflösliche Verbindung zwischen einem Mann und einer Frau von Gott im Paradies eingesetzt wurde. Er argumentierte, dass diese ursprüngliche Institution der Ehe Christus' Maßstab für die christliche Gemeinschaft sei, was eine klare Ablehnung der Polygamie einschloss. Vgl. Bullinger, In Sacrosanctum Iesu Christi Evangelium secundum Matthæum commentarii (Zürich, 1542), fol. [X].</t>
         </is>
       </c>
       <c r="E126" s="8" t="n"/>
@@ -2787,7 +2787,7 @@
     <row r="128">
       <c r="B128" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="D128" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Bullingers Vorhaben, die Vorrede seines Johanneskommentars von 1543 (HBBibl I 153) gesondert herauszugeben, wurde erst 1548 (HBBibl 1157) verwirklicht.</t>
         </is>
       </c>
       <c r="E128" s="7" t="n"/>
@@ -2808,12 +2808,12 @@
     <row r="129">
       <c r="B129" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D129" s="8" t="inlineStr">
         <is>
-          <t>Bullingers Vorhaben, die Vorrede seines Johanneskommentars von 1543 (HBBibl I 153) gesondert herauszugeben, wurde erst 1548 (HBBibl 1157) verwirklicht.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E129" s="8" t="n"/>
@@ -2824,12 +2824,12 @@
     <row r="130">
       <c r="B130" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D130" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E130" s="7" t="n"/>
@@ -2840,12 +2840,12 @@
     <row r="131">
       <c r="B131" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D131" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Bullinger bezieht sich hier auf seine geplante Vorrede zu Johannes Honterus' Werk „De iustificatione hominis Christiani“. Es handelt sich dabei um eine theologische Abhandlung, die das zentrale Thema der Rechtfertigung durch den Glauben behandelt. Bullinger wollte durch seine Vorrede möglicherweise dazu beitragen, das Werk einer breiteren Leserschaft zugänglich zu machen.</t>
         </is>
       </c>
       <c r="E131" s="8" t="n"/>
@@ -2877,7 +2877,7 @@
     <row r="133">
       <c r="B133" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="D133" s="7" t="inlineStr">
         <is>
-          <t>Nach Wasselnheim (Wasselonne, "Waßelen"; s. ebd.).</t>
+          <t>Der erwähnte "pagus" könnte sich auf ein Dorf oder eine Landgemeinde in der Nähe von Straßburg beziehen, wohin Zwingli möglicherweise gebracht wurde, um abseits der städtischen Aufregung beerdigt zu werden. Es bleibt jedoch unklar, um welchen spezifischen Ort es sich handelt, da keine weiteren Details im Brief angegeben sind.</t>
         </is>
       </c>
       <c r="E133" s="7" t="n"/>
@@ -2898,12 +2898,12 @@
     <row r="134">
       <c r="B134" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D134" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E134" s="8" t="n"/>
@@ -2914,12 +2914,12 @@
     <row r="135">
       <c r="B135" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D135" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Nach Wasselnheim (Wasselonne, "Waßelen"; s. ebd.).</t>
         </is>
       </c>
       <c r="E135" s="7" t="n"/>
@@ -2930,12 +2930,12 @@
     <row r="136">
       <c r="B136" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D136" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E136" s="8" t="n"/>
@@ -2967,7 +2967,7 @@
     <row r="138">
       <c r="B138" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="D138" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Zur Lage der Reformierten in Solothurn s. oben [Nr. 132] S. 237,3-19 und Haefliger 162-165.</t>
         </is>
       </c>
       <c r="E138" s="7" t="n"/>
@@ -2988,12 +2988,12 @@
     <row r="139">
       <c r="B139" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D139" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die "Salodorenses pii" beziehen sich wahrscheinlich auf evangelische Christen aus der Region Solothurn. Zur damaligen Zeit war Solothurn eine katholische Stadt, und die Anhänger der Reformation mussten ihre Glaubensversammlungen heimlich oder in ländlichen Gebieten außerhalb der Stadt abhalten. Die Unterstützung, die sie einem Bruder für seine Predigt boten, wäre dabei von größter Wichtigkeit gewesen, um die reformatorischen Ideen zu verbreiten.</t>
         </is>
       </c>
       <c r="E139" s="8" t="n"/>
@@ -3004,12 +3004,12 @@
     <row r="140">
       <c r="B140" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D140" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E140" s="7" t="n"/>
@@ -3020,12 +3020,12 @@
     <row r="141">
       <c r="B141" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D141" s="8" t="inlineStr">
         <is>
-          <t>Zur Lage der Reformierten in Solothurn s. oben [Nr. 132] S. 237,3-19 und Haefliger 162-165.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E141" s="8" t="n"/>
@@ -3057,7 +3057,7 @@
     <row r="143">
       <c r="B143" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3067,7 +3067,7 @@
       </c>
       <c r="D143" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E143" s="7" t="n"/>
@@ -3078,12 +3078,12 @@
     <row r="144">
       <c r="B144" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D144" s="8" t="inlineStr">
         <is>
-          <t>Myconius' Brief vom 5. Juli (Nr. 2943).</t>
+          <t>Diese Formulierung deutet darauf hin, dass Bullinger entweder Briefe oder Nachrichten von Oswald Myconius durch eine Vermittlerin erhielt. In der Korrespondenz jener Zeit wurden oft Vertrauenspersonen für die sichere Zustellung von Briefen beauftragt. Der Kontext oder die Identität der Frau bleibt aus diesem Auszug jedoch unklar.</t>
         </is>
       </c>
       <c r="E144" s="8" t="n"/>
@@ -3094,12 +3094,12 @@
     <row r="145">
       <c r="B145" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D145" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Myconius' Brief vom 5. Juli (Nr. 2943).</t>
         </is>
       </c>
       <c r="E145" s="7" t="n"/>
@@ -3110,12 +3110,12 @@
     <row r="146">
       <c r="B146" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D146" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E146" s="8" t="n"/>
@@ -3147,7 +3147,7 @@
     <row r="148">
       <c r="B148" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D148" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E148" s="7" t="n"/>
@@ -3168,12 +3168,12 @@
     <row r="149">
       <c r="B149" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D149" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Herzog Heinrich der Fromme, der Onkel der Landgräfin.</t>
         </is>
       </c>
       <c r="E149" s="8" t="n"/>
@@ -3184,12 +3184,12 @@
     <row r="150">
       <c r="B150" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D150" s="7" t="inlineStr">
         <is>
-          <t>Herzog Heinrich der Fromme, der Onkel der Landgräfin.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E150" s="7" t="n"/>
@@ -3200,12 +3200,12 @@
     <row r="151">
       <c r="B151" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D151" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der Herzog von Sachsen, Johann Friedrich I., auch bekannt als Johann der Großmütige, war ein wichtiger protestantischer Anführer in den Schmalkaldischen Kriegen. Er galt als Unterstützer der Reformatoren Martin Luther und Philipp Melanchthon und hätte seinen Einfluss wahrscheinlich genutzt, um die Interessen und Ehren seiner Familienmitglieder und der protestantischen Sache zu verteidigen.</t>
         </is>
       </c>
       <c r="E151" s="8" t="n"/>
@@ -3237,7 +3237,7 @@
     <row r="153">
       <c r="B153" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="D153" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E153" s="7" t="n"/>
@@ -3258,12 +3258,12 @@
     <row r="154">
       <c r="B154" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D154" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E154" s="8" t="n"/>
@@ -3274,12 +3274,12 @@
     <row r="155">
       <c r="B155" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D155" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Der Begriff „mansus“ bezeichnete im mittelalterlichen Rechtssystem einen landwirtschaftlichen Hof, der oft mit einer darauf befindlichen Villa verbunden war. Diese Begrifflichkeit ist typisch für das fränkische und alemannische Recht, wobei die genaue Definition und Nutzung im Laufe der Zeit variierten. Mansus wurde häufig als wirtschaftliche Einheit zur Berechnung von Abgaben und Dienstleistungen verwendet.</t>
         </is>
       </c>
       <c r="E155" s="7" t="n"/>
@@ -3327,7 +3327,7 @@
     <row r="158">
       <c r="B158" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="D158" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>In ihrer Protestation vom 4. August 1545 erneuerten die Stände der Augsburger Konfession ihre Forderungen bezüglich Friede und Recht und lehnten das Konzil von Trient ab; s. RTA JR XVI/2 1669-1672, Nr. 342.</t>
         </is>
       </c>
       <c r="E158" s="7" t="n"/>
@@ -3348,12 +3348,12 @@
     <row r="159">
       <c r="B159" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D159" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E159" s="8" t="n"/>
@@ -3364,12 +3364,12 @@
     <row r="160">
       <c r="B160" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D160" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E160" s="7" t="n"/>
@@ -3380,12 +3380,12 @@
     <row r="161">
       <c r="B161" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D161" s="8" t="inlineStr">
         <is>
-          <t>In ihrer Protestation vom 4. August 1545 erneuerten die Stände der Augsburger Konfession ihre Forderungen bezüglich Friede und Recht und lehnten das Konzil von Trient ab; s. RTA JR XVI/2 1669-1672, Nr. 342.</t>
+          <t>Diese Concessiones beziehen sich wahrscheinlich auf Zugeständnisse, die im Zuge der Verhandlungen auf Reichstagen gemacht wurden, insbesondere im Hinblick auf die religiösen und politischen Spannungen zwischen den katholischen und protestantischen Ständen im Heiligen Römischen Reich. Die Reformatoren kritisierten häufig die politischen Machenschaften, die zu ungunsten der protestantischen Sache geschahen.</t>
         </is>
       </c>
       <c r="E161" s="8" t="n"/>
@@ -3417,7 +3417,7 @@
     <row r="163">
       <c r="B163" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3427,7 +3427,7 @@
       </c>
       <c r="D163" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Es wird spekuliert, dass Haller sich hier auf einen bestimmten, möglicherweise einflussreichen Gegner oder Kritiker innerhalb der Berner Kirche bezieht. Der genaue Name wird nicht genannt, könnte jedoch in der damaligen Korrespondenz oder in den Überlieferungen über die kirchlichen Konflikte dieser Zeit zu finden sein.</t>
         </is>
       </c>
       <c r="E163" s="7" t="n"/>
@@ -3438,12 +3438,12 @@
     <row r="164">
       <c r="B164" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D164" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E164" s="8" t="n"/>
@@ -3470,12 +3470,12 @@
     <row r="166">
       <c r="B166" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D166" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E166" s="8" t="n"/>
@@ -3507,7 +3507,7 @@
     <row r="168">
       <c r="B168" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="D168" s="7" t="inlineStr">
         <is>
-          <t>Vererbliches Lehen, vgl. DRW III 95.</t>
+          <t>Das "Erblehen" (lat. Emphyteusis) beschreibt ein erbrechtliches Nutzungsverhältnis von Grundbesitz, bei dem der Empfänger das Land gegen einen vereinbarten Zins oder Verpflichtung dauerhaft nutzen kann. Dieses Rechtsinstitut war im Mittelalter weit verbreitet und ermöglichte es, Land langfristig zu bewirtschaften, ohne das Eigentum daran zu besitzen. Das Recht ging bei Erbschaft an die Nachkommen über, was es stabil und attraktiv für die Landwirtschaft und Siedlungsentwicklung machte.</t>
         </is>
       </c>
       <c r="E168" s="7" t="n"/>
@@ -3528,12 +3528,12 @@
     <row r="169">
       <c r="B169" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D169" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E169" s="8" t="n"/>
@@ -3544,12 +3544,12 @@
     <row r="170">
       <c r="B170" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D170" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E170" s="7" t="n"/>
@@ -3560,12 +3560,12 @@
     <row r="171">
       <c r="B171" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D171" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vererbliches Lehen, vgl. DRW III 95.</t>
         </is>
       </c>
       <c r="E171" s="8" t="n"/>
@@ -3597,7 +3597,7 @@
     <row r="173">
       <c r="B173" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="D173" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E173" s="7" t="n"/>
@@ -3634,12 +3634,12 @@
     <row r="175">
       <c r="B175" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D175" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Unklar bleibt, welcher Jacobi a Madiis hier genau gemeint ist. Der Brief verweist jedoch auf eine engere Verbindung zwischen Bullinger und der Familie Madi, die in verschiedenen Funktionen in Zürich tätig waren. Siehe dazu auch Müller, „Die Zürcher Familie Madi und ihre Verbindungen“, in: Zürcher Jahrbuch für Regionalgeschichte, 1987, S. 145-160.</t>
         </is>
       </c>
       <c r="E175" s="7" t="n"/>
@@ -3650,12 +3650,12 @@
     <row r="176">
       <c r="B176" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D176" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E176" s="8" t="n"/>
@@ -3687,7 +3687,7 @@
     <row r="178">
       <c r="B178" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="D178" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Vgl. dazu Bullingers Antwortbrief an Bucer, datiert auf den 20. Dezember 1534, in dem Bullinger auf die von Bucer erwähnte Confessio Bezug nimmt und seine Ansichten zur Abendmahlsfrage darlegt. (Siehe &lt;ref target="file10523"&gt;Nr. 476&lt;/ref&gt; in diesem Band.)</t>
         </is>
       </c>
       <c r="E178" s="7" t="n"/>
@@ -3708,12 +3708,12 @@
     <row r="179">
       <c r="B179" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D179" s="8" t="inlineStr">
         <is>
-          <t>Die schon in Anm. 2 erwähnte Nr. 463.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E179" s="8" t="n"/>
@@ -3724,12 +3724,12 @@
     <row r="180">
       <c r="B180" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D180" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E180" s="7" t="n"/>
@@ -3740,12 +3740,12 @@
     <row r="181">
       <c r="B181" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D181" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die schon in Anm. 2 erwähnte Nr. 463.</t>
         </is>
       </c>
       <c r="E181" s="8" t="n"/>
@@ -3777,7 +3777,7 @@
     <row r="183">
       <c r="B183" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="D183" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E183" s="7" t="n"/>
@@ -3798,12 +3798,12 @@
     <row r="184">
       <c r="B184" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D184" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E184" s="8" t="n"/>
@@ -3830,12 +3830,12 @@
     <row r="186">
       <c r="B186" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D186" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Konrad Pellikan (1478–1556) war ein bedeutender Reformator und Hebräist, der in Zürich wirkte. Seine umfassende Arbeit an den "Kommentarien zu den Büchern der Bibel", die aus sieben Bänden bestand, prägte die reformatorische Bibelauslegung entscheidend. Pellikans detaillierte Kommentare galten als wertvolle Quelle für Theologen und Geistliche seiner Zeit.</t>
         </is>
       </c>
       <c r="E186" s="8" t="n"/>
@@ -3867,7 +3867,7 @@
     <row r="188">
       <c r="B188" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -3877,7 +3877,7 @@
       </c>
       <c r="D188" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Johannes und Justus Vulteius.</t>
         </is>
       </c>
       <c r="E188" s="7" t="n"/>
@@ -3888,12 +3888,12 @@
     <row r="189">
       <c r="B189" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D189" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E189" s="8" t="n"/>
@@ -3904,12 +3904,12 @@
     <row r="190">
       <c r="B190" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D190" s="7" t="inlineStr">
         <is>
-          <t>Johannes und Justus Vulteius.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E190" s="7" t="n"/>
@@ -3920,12 +3920,12 @@
     <row r="191">
       <c r="B191" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D191" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die zwei erwähnten Jugendlichen könnten Studenten oder Lehrlinge gewesen sein, die von Marburg nach Zürich reisten. Eine genauere Identifikation ist ohne zusätzliche Quellen schwierig. Eventuell handelt es sich um Theologiestudenten, die bei Heinrich Bullinger studieren oder sich ausbilden lassen wollten.</t>
         </is>
       </c>
       <c r="E191" s="8" t="n"/>
@@ -3957,7 +3957,7 @@
     <row r="193">
       <c r="B193" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="D193" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E193" s="7" t="n"/>
@@ -3994,12 +3994,12 @@
     <row r="195">
       <c r="B195" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D195" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E195" s="7" t="n"/>
@@ -4010,12 +4010,12 @@
     <row r="196">
       <c r="B196" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D196" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Anna Adlischweiler, Heinrich Bullingers Ehefrau seit 1529, war die Tochter von Rudolf Adlischweiler. Die Ehe der beiden galt als harmonisch und von tiefem gegenseitigem Respekt geprägt. Anna unterstützte Bullinger in seinem pastoralen und theologischen Wirken und wohnte mit ihm in Zürich, wo sie gemeinsam eine große Familie großzogen.</t>
         </is>
       </c>
       <c r="E196" s="8" t="n"/>
@@ -4047,7 +4047,7 @@
     <row r="198">
       <c r="B198" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -4057,7 +4057,7 @@
       </c>
       <c r="D198" s="7" t="inlineStr">
         <is>
-          <t>Landgräfin Christine von Hessen.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E198" s="7" t="n"/>
@@ -4068,12 +4068,12 @@
     <row r="199">
       <c r="B199" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D199" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Landgräfin Christine von Hessen.</t>
         </is>
       </c>
       <c r="E199" s="8" t="n"/>
@@ -4084,12 +4084,12 @@
     <row r="200">
       <c r="B200" t="inlineStr">
         <is>
-          <t>model1</t>
+          <t>fake_model1</t>
         </is>
       </c>
       <c r="D200" s="7" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E200" s="7" t="n"/>
@@ -4100,12 +4100,12 @@
     <row r="201">
       <c r="B201" t="inlineStr">
         <is>
-          <t>model3</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D201" s="8" t="inlineStr">
         <is>
-          <t>Lorem ipsum dolor sit amet</t>
+          <t>Die Erwähnung einer "altera" bezieht sich vermutlich auf eine weitere im Brief erwähnte Person im Umfeld des Landgrafen von Hessen. In diesem Kontext ist es möglich, dass "altera" auf eine andere Geliebte oder sogar Ehefrau bezogen ist, was im historischen Hintergrund der Landgrafen von Hessen, insbesondere im Zusammenhang mit landgräflichen Familienstreitigkeiten und der komplexen Heiratspolitik, nicht selten war. Eine detaillierte Identifizierung erfordert jedoch umfassendere historische Recherchen in den familiären Verflechtungen des Landgrafenhofes dieser Zeit.</t>
         </is>
       </c>
       <c r="E201" s="8" t="n"/>

</xml_diff>

<commit_message>
add the llama-8B to the eval excel sheet
</commit_message>
<xml_diff>
--- a/evaluate/human_eval/evaluation_form_v1.xlsx
+++ b/evaluate/human_eval/evaluation_form_v1.xlsx
@@ -558,12 +558,12 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>Vgl. 1Kor 7, 25.</t>
+          <t>&lt;p&gt;4, 1.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E4" s="8" t="n"/>
@@ -574,12 +574,12 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1Kor 7, 25.</t>
         </is>
       </c>
       <c r="E5" s="7" t="n"/>
@@ -627,7 +627,7 @@
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -637,7 +637,7 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>Vgl. 1 Kor 7,2. 28. 36.</t>
+          <t>Bullinger verteidigt hier die Ehe als einen göttlich eingesetzten Stand, der nicht per se sündhaft ist. Dies verweist auf die reformatorische Ablehnung der klösterlichen Gelübde und unterstreicht die Bedeutung der Ehe als gleichwertige und tugendhafte Lebensform im Gegensatz zum klösterlichen Leben.</t>
         </is>
       </c>
       <c r="E8" s="7" t="n"/>
@@ -664,12 +664,12 @@
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1 Kor 7,2. 28. 36.</t>
         </is>
       </c>
       <c r="E10" s="7" t="n"/>
@@ -680,12 +680,12 @@
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>Bullinger verteidigt hier die Ehe als einen göttlich eingesetzten Stand, der nicht per se sündhaft ist. Dies verweist auf die reformatorische Ablehnung der klösterlichen Gelübde und unterstreicht die Bedeutung der Ehe als gleichwertige und tugendhafte Lebensform im Gegensatz zum klösterlichen Leben.</t>
+          <t>So sind sy nitt schwach, sunder wellend mitt gwallt verergeret sin: 1. Timoth. 4 [6].</t>
         </is>
       </c>
       <c r="E11" s="8" t="n"/>
@@ -717,7 +717,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="D13" s="7" t="inlineStr">
         <is>
-          <t>Siehe oben Anm. 53.</t>
+          <t>Da wir gesternn furtgedruckt, Nr. 25.</t>
         </is>
       </c>
       <c r="E13" s="7" t="n"/>
@@ -738,12 +738,12 @@
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Siehe oben Anm. 53.</t>
         </is>
       </c>
       <c r="E14" s="8" t="n"/>
@@ -754,12 +754,12 @@
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D15" s="7" t="inlineStr">
         <is>
-          <t>„Vortgetruckt“ in diesem Kontext bedeutet einen militärischen Vorstoß oder Angriff. Der Begriff wurde häufig verwendet, um den Vormarsch oder das Fortschreiten von Truppen in Richtung des Feindes zu beschreiben. Am 2. September 1546 wurde ein Angriff auf die feindlichen Positionen ausgeführt, der als erfolgreich beschrieben wird, indem er erheblichen Schaden verursachte.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E15" s="7" t="n"/>
@@ -770,12 +770,12 @@
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>„Vortgetruckt“ in diesem Kontext bedeutet einen militärischen Vorstoß oder Angriff. Der Begriff wurde häufig verwendet, um den Vormarsch oder das Fortschreiten von Truppen in Richtung des Feindes zu beschreiben. Am 2. September 1546 wurde ein Angriff auf die feindlichen Positionen ausgeführt, der als erfolgreich beschrieben wird, indem er erheblichen Schaden verursachte.</t>
         </is>
       </c>
       <c r="E16" s="8" t="n"/>
@@ -807,7 +807,7 @@
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -860,12 +860,12 @@
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Das Schreiben, das Blarer (als Boten der Neun Orte) von den V Orten erhalten hatte, ist nicht erhalten; die hier angegebene Stelle ist aber durch den Eintrag in Zürich StA, A. A. (s. Anm. 1) nachgewiesen.</t>
         </is>
       </c>
       <c r="E21" s="8" t="n"/>
@@ -897,7 +897,7 @@
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="D23" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>König Ferdinand und Christoph von Württemberg einigten sich nicht, vgl. unten Z. 77-81 und Wille 120-130. 137f. 141-144.</t>
         </is>
       </c>
       <c r="E23" s="7" t="n"/>
@@ -918,12 +918,12 @@
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>König Ferdinand und Christoph von Württemberg einigten sich nicht, vgl. unten Z. 77-81 und Wille 120-130. 137f. 141-144.</t>
+          <t>Die Verhandlungen zwischen der königlichen Majestät und Herzog Christoph von Württemberg bezogen sich auf die Rückerlangung seines Herzogtums, das sein Vater im Jahre 1519 verloren hatte. Die Reichspolitik war durch die Absichten des Kaisers Karl V. geprägt, der die Unterstützung der deutschen Fürsten benötigte, um seine Macht im Reich zu sichern.</t>
         </is>
       </c>
       <c r="E24" s="8" t="n"/>
@@ -934,12 +934,12 @@
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D25" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Sic, sic, mi Bullingere, vix adhuc in lucem ędito Christo apud Gallos Herodes insidiatur, ut perdat.</t>
         </is>
       </c>
       <c r="E25" s="7" t="n"/>
@@ -950,12 +950,12 @@
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Die Verhandlungen zwischen der königlichen Majestät und Herzog Christoph von Württemberg bezogen sich auf die Rückerlangung seines Herzogtums, das sein Vater im Jahre 1519 verloren hatte. Die Reichspolitik war durch die Absichten des Kaisers Karl V. geprägt, der die Unterstützung der deutschen Fürsten benötigte, um seine Macht im Reich zu sichern.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E26" s="8" t="n"/>
@@ -987,7 +987,7 @@
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="D28" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>&lt;persName ref="p1387" cert="high"&gt;Thomas Gaßner&lt;/persName&gt;. - Der Brief Gaßners an &lt;persName ref="p8071" cert="high"&gt;Vogler&lt;/persName&gt; ist nicht erhalten.</t>
         </is>
       </c>
       <c r="E28" s="7" t="n"/>
@@ -1077,7 +1077,7 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D33" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Hand zu wordt: Sie geben vor.</t>
         </is>
       </c>
       <c r="E33" s="7" t="n"/>
@@ -1098,12 +1098,12 @@
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Die Redewendung "Hand zu wordt" bedeutet, dass Taten den Worten folgen müssen oder dass Versprechen in die Tat umgesetzt werden sollen. In diesem Kontext betont Johannes Haab möglicherweise die Notwendigkeit, entschlossen zu handeln, anstatt nur darüber zu sprechen, in eine militärische Auseinandersetzung einzutreten.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E34" s="8" t="n"/>
@@ -1114,12 +1114,12 @@
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D35" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Es fehlt der entsprechende Aufzeichnung.</t>
         </is>
       </c>
       <c r="E35" s="7" t="n"/>
@@ -1130,12 +1130,12 @@
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D36" s="8" t="inlineStr">
         <is>
-          <t>Hand zu wordt: Sie geben vor.</t>
+          <t>Die Redewendung "Hand zu wordt" bedeutet, dass Taten den Worten folgen müssen oder dass Versprechen in die Tat umgesetzt werden sollen. In diesem Kontext betont Johannes Haab möglicherweise die Notwendigkeit, entschlossen zu handeln, anstatt nur darüber zu sprechen, in eine militärische Auseinandersetzung einzutreten.</t>
         </is>
       </c>
       <c r="E36" s="8" t="n"/>
@@ -1188,12 +1188,12 @@
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D39" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>&lt;persName ref="p4091" cert="high"&gt;Zwinglis&lt;/persName&gt; Kommentar zum Matthäus, &lt;bibl&gt;Zürich StA&lt;/bibl&gt; Bollingeram I 144, erschien im August 1542 bei &lt;persName ref="p1227" cert="high"&gt;Christoph Froschauer&lt;/persName&gt; in Zürich.</t>
         </is>
       </c>
       <c r="E39" s="8" t="n"/>
@@ -1204,12 +1204,12 @@
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D40" s="7" t="inlineStr">
         <is>
-          <t>Heinrich Bullingers Werk „De unico et aeterno Testamento Dei“ wurde 1534 veröffentlicht. In diesem Werk verteidigt Bullinger die Einheit und Kontinuität des göttlichen Testaments und behandelt Aspekte der Theologie, die auch im Diskurs gegen die Täufer von Bedeutung waren.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E40" s="7" t="n"/>
@@ -1220,12 +1220,12 @@
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D41" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Heinrich Bullingers Werk „De unico et aeterno Testamento Dei“ wurde 1534 veröffentlicht. In diesem Werk verteidigt Bullinger die Einheit und Kontinuität des göttlichen Testaments und behandelt Aspekte der Theologie, die auch im Diskurs gegen die Täufer von Bedeutung waren.</t>
         </is>
       </c>
       <c r="E41" s="8" t="n"/>
@@ -1257,7 +1257,7 @@
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Vgl. Lang, aaO, f. Biij,r.-v.; und [Enzinas], aaO, S. 137-142, wo das Ganze noch ausführlicher geschildert wird.</t>
         </is>
       </c>
       <c r="E43" s="7" t="n"/>
@@ -1278,12 +1278,12 @@
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D44" s="8" t="inlineStr">
         <is>
-          <t>Vgl. Lang, aaO, f. Biij,r.-v.; und [Enzinas], aaO, S. 137-142, wo das Ganze noch ausführlicher geschildert wird.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E44" s="8" t="n"/>
@@ -1294,12 +1294,12 @@
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D45" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Der Mord an Johannes Diacius, einem Anhänger der Reformation, durch seinen eigenen Bruder Alphonsus Diazius, einem katholischen Richter, ist ein historisches Ereignis, das die konfessionellen Spannungen der Zeit widerspiegelt. Diese Tat geschah 1546 in Augsburg, während einer Epoche, in der reformatorisches und katholisches Gedankengut häufig zu offenen Konflikten führte. Die Schilderung des Vorfalls in diesem Brief zeigt die Dramatik und die Gefährdung derjenigen, die sich zur Reformation bekannten. Siehe dazu auch die Anmerkungen von Heinrich Bullinger in seinen Aufzeichnungen bezüglich der Konsequenzen für die beteiligten Personen, insbesondere die Maßnahmen gegen Alphonsus nach seiner Festnahme in Innsbruck.</t>
         </is>
       </c>
       <c r="E45" s="7" t="n"/>
@@ -1310,12 +1310,12 @@
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D46" s="8" t="inlineStr">
         <is>
-          <t>Der Mord an Johannes Diacius, einem Anhänger der Reformation, durch seinen eigenen Bruder Alphonsus Diazius, einem katholischen Richter, ist ein historisches Ereignis, das die konfessionellen Spannungen der Zeit widerspiegelt. Diese Tat geschah 1546 in Augsburg, während einer Epoche, in der reformatorisches und katholisches Gedankengut häufig zu offenen Konflikten führte. Die Schilderung des Vorfalls in diesem Brief zeigt die Dramatik und die Gefährdung derjenigen, die sich zur Reformation bekannten. Siehe dazu auch die Anmerkungen von Heinrich Bullinger in seinen Aufzeichnungen bezüglich der Konsequenzen für die beteiligten Personen, insbesondere die Maßnahmen gegen Alphonsus nach seiner Festnahme in Innsbruck.</t>
+          <t>&lt;persName ref="p5481" cert="high"&gt;Joärg&lt;/persName&gt; von &lt;placeName ref="l2259" cert="high"&gt;Pethmes&lt;/placeName&gt; verletzte den &lt;persName ref="p4631" cert="high"&gt;Joannes Diacius&lt;/persName&gt;, der im &lt;placeName ref="l337" cert="high"&gt;Nuwenburg&lt;/placeName&gt; ermordt wurde.</t>
         </is>
       </c>
       <c r="E46" s="8" t="n"/>
@@ -1347,7 +1347,7 @@
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="D48" s="7" t="inlineStr">
         <is>
-          <t>Rohrenfels (Lkr. Neuburg-Schrobenhausen), südlich von Neuburg a.d. Donau.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E48" s="7" t="n"/>
@@ -1368,12 +1368,12 @@
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D49" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Rohrenfels (Lkr. Neuburg-Schrobenhausen), südlich von Neuburg a.d. Donau.</t>
         </is>
       </c>
       <c r="E49" s="8" t="n"/>
@@ -1384,12 +1384,12 @@
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D50" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Rornfels (möglicherweise ein Missverständnis oder eine Schreibvariante für die Ortschaft oder Region Rornfels/Rorhbach, die nicht eindeutig identifiziert werden kann).</t>
         </is>
       </c>
       <c r="E50" s="7" t="n"/>
@@ -1400,12 +1400,12 @@
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D51" s="8" t="inlineStr">
         <is>
-          <t>Rornfels (möglicherweise ein Missverständnis oder eine Schreibvariante für die Ortschaft oder Region Rornfels/Rorhbach, die nicht eindeutig identifiziert werden kann).</t>
+          <t>dieser Briefe (mit Singularbedeutung).</t>
         </is>
       </c>
       <c r="E51" s="8" t="n"/>
@@ -1437,7 +1437,7 @@
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D53" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Siehe dazu Nr. 2452, Anm. 2.</t>
         </is>
       </c>
       <c r="E53" s="7" t="n"/>
@@ -1474,12 +1474,12 @@
     <row r="55">
       <c r="B55" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D55" s="7" t="inlineStr">
         <is>
-          <t>Siehe dazu Nr. 2452, Anm. 2.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E55" s="7" t="n"/>
@@ -1490,12 +1490,12 @@
     <row r="56">
       <c r="B56" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D56" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>&lt;persName ref="p18312" cert="high"&gt;Ulrich von Württemberg&lt;/persName&gt;. - Siehe &lt;bibl&gt;HBBW&lt;/bibl&gt; XVI 399, 12.</t>
         </is>
       </c>
       <c r="E56" s="8" t="n"/>
@@ -1527,7 +1527,7 @@
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1548,12 +1548,12 @@
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D59" s="8" t="inlineStr">
         <is>
-          <t>Der eingefügte Zettel enthält zusätzliche Informationen oder spezifische Details, die nicht im Haupttext des Briefes enthalten sind. Solche Einlagen waren üblich, um vertrauliche oder detaillierte Anweisungen zu geben. Es war nicht unüblich, dass vertrauliche Mitteilungen oder wichtige Informationen in separaten Notizen übermittelt wurden, die dann später zerstört oder anderweitig behandelt wurden, um die Vertraulichkeit zu wahren.</t>
+          <t>Vermutlich waren es diese beiden Dokumente, die Blarer am 26. Dezember zurückverlangte; s. oben .</t>
         </is>
       </c>
       <c r="E59" s="8" t="n"/>
@@ -1564,12 +1564,12 @@
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D60" s="7" t="inlineStr">
         <is>
-          <t>Vermutlich waren es diese beiden Dokumente, die Blarer am 26. Dezember zurückverlangte; s. oben .</t>
+          <t>Zu verstehen: das er schreibe.</t>
         </is>
       </c>
       <c r="E60" s="7" t="n"/>
@@ -1580,12 +1580,12 @@
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D61" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Der eingefügte Zettel enthält zusätzliche Informationen oder spezifische Details, die nicht im Haupttext des Briefes enthalten sind. Solche Einlagen waren üblich, um vertrauliche oder detaillierte Anweisungen zu geben. Es war nicht unüblich, dass vertrauliche Mitteilungen oder wichtige Informationen in separaten Notizen übermittelt wurden, die dann später zerstört oder anderweitig behandelt wurden, um die Vertraulichkeit zu wahren.</t>
         </is>
       </c>
       <c r="E61" s="8" t="n"/>
@@ -1617,7 +1617,7 @@
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1638,12 +1638,12 @@
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D64" s="8" t="inlineStr">
         <is>
-          <t>Die "Ordnung der reisglöffen" bezieht sich auf die Disposition oder den Marschbefehl der Berner Truppen, welcher offensichtlich bestimmte Voraussetzungen für ihre Rückkehr oder den weiteren Verlauf ihrer Mission forderte. Es könnte sich um logistische, taktische oder diplomatische Anweisungen gehandelt haben.</t>
+          <t>Ein unbekannter Bote des Landvogts von &lt;placeName ref="l167" cert="high"&gt;Genf&lt;/placeName&gt;.</t>
         </is>
       </c>
       <c r="E64" s="8" t="n"/>
@@ -1654,12 +1654,12 @@
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D65" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Seit 1529 bzw. 1530 galt in Bern ein strenges Pensionen- und Reislaufverbot (SSRQ Bern I 11 362-368, vgl. Z XI 480, Anm. 4).</t>
         </is>
       </c>
       <c r="E65" s="7" t="n"/>
@@ -1670,12 +1670,12 @@
     <row r="66">
       <c r="B66" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D66" s="8" t="inlineStr">
         <is>
-          <t>Seit 1529 bzw. 1530 galt in Bern ein strenges Pensionen- und Reislaufverbot (SSRQ Bern I 11 362-368, vgl. Z XI 480, Anm. 4).</t>
+          <t>Die "Ordnung der reisglöffen" bezieht sich auf die Disposition oder den Marschbefehl der Berner Truppen, welcher offensichtlich bestimmte Voraussetzungen für ihre Rückkehr oder den weiteren Verlauf ihrer Mission forderte. Es könnte sich um logistische, taktische oder diplomatische Anweisungen gehandelt haben.</t>
         </is>
       </c>
       <c r="E66" s="8" t="n"/>
@@ -1707,7 +1707,7 @@
     <row r="68">
       <c r="B68" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="D68" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Die katholischen Orte, die mit Zürich den Thurgau verwalteten.</t>
         </is>
       </c>
       <c r="E68" s="7" t="n"/>
@@ -1728,7 +1728,7 @@
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D69" s="8" t="inlineStr">
@@ -1744,12 +1744,12 @@
     <row r="70">
       <c r="B70" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D70" s="7" t="inlineStr">
         <is>
-          <t>Die katholischen Orte, die mit Zürich den Thurgau verwalteten.</t>
+          <t>&lt;persName ref="p199" cert="high"&gt;Rudolf Schwyzer&lt;/persName&gt;.</t>
         </is>
       </c>
       <c r="E70" s="7" t="n"/>
@@ -1797,7 +1797,7 @@
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D73" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Dieser Abschnitt ist Teil der strategischen Überlegungen im Zusammenhang mit den Auseinandersetzungen des Schmalkaldischen Krieges (1546–1547), bei dem der Kaiser versuchte, seine Kontrolle über die protestantischen Fürsten im Heiligen Römischen Reich auszudehnen. Der von Johannes Gast erwähnte „Weg, den die Niderlender heruff synt zogen“, könnte auf die Bewegungen der kaiserlichen Truppen hinweisen, die aus den Niederlanden kommend, den protestantischen Gebieten Deutschlands entgegenzogen, um diese zu unterwerfen.</t>
         </is>
       </c>
       <c r="E73" s="7" t="n"/>
@@ -1818,12 +1818,12 @@
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D74" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Zu dieser Route des niederländischen Heeres unter Maximilian von Egmont, Graf von Büren, auf dem Weg zum kaiserlichen Lager s. HBBW XVII 415, Anm. 43.</t>
         </is>
       </c>
       <c r="E74" s="8" t="n"/>
@@ -1834,12 +1834,12 @@
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D75" s="7" t="inlineStr">
         <is>
-          <t>Zu dieser Route des niederländischen Heeres unter Maximilian von Egmont, Graf von Büren, auf dem Weg zum kaiserlichen Lager s. HBBW XVII 415, Anm. 43.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E75" s="7" t="n"/>
@@ -1850,12 +1850,12 @@
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D76" s="8" t="inlineStr">
         <is>
-          <t>Dieser Abschnitt ist Teil der strategischen Überlegungen im Zusammenhang mit den Auseinandersetzungen des Schmalkaldischen Krieges (1546–1547), bei dem der Kaiser versuchte, seine Kontrolle über die protestantischen Fürsten im Heiligen Römischen Reich auszudehnen. Der von Johannes Gast erwähnte „Weg, den die Niderlender heruff synt zogen“, könnte auf die Bewegungen der kaiserlichen Truppen hinweisen, die aus den Niederlanden kommend, den protestantischen Gebieten Deutschlands entgegenzogen, um diese zu unterwerfen.</t>
+          <t>Mit Brief &lt;ref target="file12672"&gt;Nr. 2625&lt;/ref&gt; vom 14. Oktober. - Vgl. ferner &lt;bibl&gt;HBBW&lt;/bibl&gt; XVII 250,42, und 261,1-6.</t>
         </is>
       </c>
       <c r="E76" s="8" t="n"/>
@@ -1887,7 +1887,7 @@
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="D78" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>nieman hochen: keine hochrangige Persönlichkeit.</t>
         </is>
       </c>
       <c r="E78" s="7" t="n"/>
@@ -1940,12 +1940,12 @@
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D81" s="8" t="inlineStr">
         <is>
-          <t>nieman hochen: keine hochrangige Persönlichkeit.</t>
+          <t>hochmüthig.</t>
         </is>
       </c>
       <c r="E81" s="8" t="n"/>
@@ -1977,7 +1977,7 @@
     <row r="83">
       <c r="B83" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="D83" s="7" t="inlineStr">
         <is>
-          <t>ain mittlyden gebärdet: Anteilnahme bekundet.</t>
+          <t>Ein "nachpurlichs mittlyden gebärdet" bezieht sich auf ein nachbarliches Mitleid, das die Ratsherren von Lindau gegenüber den Empfängern des Mandats kundtaten. Diese Formulierung zeigt, dass die Ratsherren bedauerten, ein Mandat überbracht zu haben, wahrscheinlich im Rahmen von politischen Maßnahmen oder Konflikten, die nicht in ihrem Einflussbereich lagen und dennoch umgesetzt werden mussten.</t>
         </is>
       </c>
       <c r="E83" s="7" t="n"/>
@@ -1998,12 +1998,12 @@
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D84" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>&lt;persName ref="p182" cert="high"&gt;Gabriel Arnold&lt;/persName&gt;.</t>
         </is>
       </c>
       <c r="E84" s="8" t="n"/>
@@ -2030,12 +2030,12 @@
     <row r="86">
       <c r="B86" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D86" s="8" t="inlineStr">
         <is>
-          <t>Ein "nachpurlichs mittlyden gebärdet" bezieht sich auf ein nachbarliches Mitleid, das die Ratsherren von Lindau gegenüber den Empfängern des Mandats kundtaten. Diese Formulierung zeigt, dass die Ratsherren bedauerten, ein Mandat überbracht zu haben, wahrscheinlich im Rahmen von politischen Maßnahmen oder Konflikten, die nicht in ihrem Einflussbereich lagen und dennoch umgesetzt werden mussten.</t>
+          <t>ain mittlyden gebärdet: Anteilnahme bekundet.</t>
         </is>
       </c>
       <c r="E86" s="8" t="n"/>
@@ -2067,7 +2067,7 @@
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="D88" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>dort, nördlich von Basel.</t>
         </is>
       </c>
       <c r="E88" s="7" t="n"/>
@@ -2088,12 +2088,12 @@
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D89" s="8" t="inlineStr">
         <is>
-          <t>"Daniden" scheint im Kontext des Briefes das Synonym für eine Begräbnisstätte zu sein, welches sich möglicherweise auf eine lokale oder altsprachliche Eigenheit bezieht. Ein "Schwäher" (Schwiegervater) hätte demnach eine von der reformierten Ordnung abweichende Bestattung arrangiert, wobei Elemente wie Kerzen, Weihwasser und Gesang verwendet werden. Solche Rituale waren aus reformatorischer Sicht umstritten. Beachten Sie, dass solche Begräbnisse Teil der umfänglicheren Konfessionskonflikte der Zeit waren, in denen die alten katholischen Bräuche stark in Frage gestellt wurden.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E89" s="8" t="n"/>
@@ -2104,12 +2104,12 @@
     <row r="90">
       <c r="B90" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D90" s="7" t="inlineStr">
         <is>
-          <t>dort, nördlich von Basel.</t>
+          <t>"Daniden" scheint im Kontext des Briefes das Synonym für eine Begräbnisstätte zu sein, welches sich möglicherweise auf eine lokale oder altsprachliche Eigenheit bezieht. Ein "Schwäher" (Schwiegervater) hätte demnach eine von der reformierten Ordnung abweichende Bestattung arrangiert, wobei Elemente wie Kerzen, Weihwasser und Gesang verwendet werden. Solche Rituale waren aus reformatorischer Sicht umstritten. Beachten Sie, dass solche Begräbnisse Teil der umfänglicheren Konfessionskonflikte der Zeit waren, in denen die alten katholischen Bräuche stark in Frage gestellt wurden.</t>
         </is>
       </c>
       <c r="E90" s="7" t="n"/>
@@ -2120,12 +2120,12 @@
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D91" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Mit Brief &lt;ref target="file12672"&gt;Nr. 2625&lt;/ref&gt; vom 14. Oktober. - Vgl. ferner &lt;bibl&gt;HBBW&lt;/bibl&gt; XVII 250,42, und 261,1-6.</t>
         </is>
       </c>
       <c r="E91" s="8" t="n"/>
@@ -2157,7 +2157,7 @@
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D93" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>(Er) solle (sie).</t>
         </is>
       </c>
       <c r="E93" s="7" t="n"/>
@@ -2194,12 +2194,12 @@
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D95" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Gemeint ist: Solle.</t>
         </is>
       </c>
       <c r="E95" s="7" t="n"/>
@@ -2210,12 +2210,12 @@
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D96" s="8" t="inlineStr">
         <is>
-          <t>(Er) solle (sie).</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E96" s="8" t="n"/>
@@ -2300,12 +2300,12 @@
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D101" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>mitwoch vor letare anno 1534.</t>
         </is>
       </c>
       <c r="E101" s="8" t="n"/>
@@ -2337,7 +2337,7 @@
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D103" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Der Ausdruck "carnis internitionem spiritus alimentum esse" im Brief von Gervasius Schuler an Heinrich Bullinger spiegelt eine gängige theologische Sichtweise der Reformationszeit wider, die aus der paulinischen Theologie der Kreuzigung des Fleisches (vgl. Galater 5,24) abgeleitet ist und im Kontext der asketischen Praxis interpretiert wird. Das Töten des Fleisches wird als Nahrung für den Geist angesehen, was den Wert des Leidens im Streben nach spiritueller Erbauung und Nähe zu Gott betont.</t>
         </is>
       </c>
       <c r="E103" s="7" t="n"/>
@@ -2358,12 +2358,12 @@
     <row r="104">
       <c r="B104" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D104" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Vgl. 1 Kor 5,5.</t>
         </is>
       </c>
       <c r="E104" s="8" t="n"/>
@@ -2374,12 +2374,12 @@
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D105" s="7" t="inlineStr">
         <is>
-          <t>Vgl. 1 Kor 5,5.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E105" s="7" t="n"/>
@@ -2390,12 +2390,12 @@
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D106" s="8" t="inlineStr">
         <is>
-          <t>Der Ausdruck "carnis internitionem spiritus alimentum esse" im Brief von Gervasius Schuler an Heinrich Bullinger spiegelt eine gängige theologische Sichtweise der Reformationszeit wider, die aus der paulinischen Theologie der Kreuzigung des Fleisches (vgl. Galater 5,24) abgeleitet ist und im Kontext der asketischen Praxis interpretiert wird. Das Töten des Fleisches wird als Nahrung für den Geist angesehen, was den Wert des Leidens im Streben nach spiritueller Erbauung und Nähe zu Gott betont.</t>
+          <t>Vgl. Adagia, 1, 2, 32 (&lt;bibl&gt;LB&lt;/bibl&gt; I 137).</t>
         </is>
       </c>
       <c r="E106" s="8" t="n"/>
@@ -2448,12 +2448,12 @@
     <row r="109">
       <c r="B109" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D109" s="8" t="inlineStr">
         <is>
-          <t>Vgl. Röm 14, 5.</t>
+          <t>Die Redewendung "abundare in sensu suo" stammt aus der Vulgata, dem lateinischen Text der Bibel, und bedeutet wörtlich "in seiner eigenen Meinung reichlich sein". Im übertragenen Sinne wird es als Aufforderung verstanden, bei der eigenen Meinung zu bleiben, ohne sich von äußeren Einflüssen oder Widerspruch beeindrucken zu lassen. Diese Redewendung drückt eine gewisse Toleranz gegenüber unterschiedlichen Ansichten aus und findet sich oft in theologischen Diskussionen der Reformationszeit.</t>
         </is>
       </c>
       <c r="E109" s="8" t="n"/>
@@ -2464,12 +2464,12 @@
     <row r="110">
       <c r="B110" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D110" s="7" t="inlineStr">
         <is>
-          <t>Die Redewendung "abundare in sensu suo" stammt aus der Vulgata, dem lateinischen Text der Bibel, und bedeutet wörtlich "in seiner eigenen Meinung reichlich sein". Im übertragenen Sinne wird es als Aufforderung verstanden, bei der eigenen Meinung zu bleiben, ohne sich von äußeren Einflüssen oder Widerspruch beeindrucken zu lassen. Diese Redewendung drückt eine gewisse Toleranz gegenüber unterschiedlichen Ansichten aus und findet sich oft in theologischen Diskussionen der Reformationszeit.</t>
+          <t>Zu vermuten ist, daß Bullinger den Baslern die Antwort &lt;persName ref="p1365" cert="high"&gt;Grynaeus&lt;/persName&gt; mitgetheilt hatte.</t>
         </is>
       </c>
       <c r="E110" s="7" t="n"/>
@@ -2480,12 +2480,12 @@
     <row r="111">
       <c r="B111" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D111" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Vgl. Röm 14, 5.</t>
         </is>
       </c>
       <c r="E111" s="8" t="n"/>
@@ -2517,7 +2517,7 @@
     <row r="113">
       <c r="B113" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="D113" s="7" t="inlineStr">
         <is>
-          <t>In diesem Abschnitt des Briefes betont Bullinger seine Unvoreingenommenheit und die Bereitschaft zur Zusammenarbeit. Das Wort "praeiuditio" steht hier für Vorurteil oder Voreingenommenheit. Er drückt aus, dass seine Überlegungen und Absichten frei von persönlichen Vorurteilen sind. Angesichts ihrer gemeinsamen Anstrengungen unterstreicht er die Hoffnung auf das Beste, insbesondere im Hinblick auf die Zusammenarbeit mit Ambrosius Blarer und Simon Grynaeus. Diese Passage soll Vertrauen und Einigkeit in der theologischen Diskussion stärken.</t>
+          <t>Vgl. &lt;bibl&gt;HBBW&lt;/bibl&gt; II 144, Anm. 20.</t>
         </is>
       </c>
       <c r="E113" s="7" t="n"/>
@@ -2538,7 +2538,7 @@
     <row r="114">
       <c r="B114" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D114" s="8" t="inlineStr">
@@ -2554,12 +2554,12 @@
     <row r="115">
       <c r="B115" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D115" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>1 Tim 5, 21.</t>
         </is>
       </c>
       <c r="E115" s="7" t="n"/>
@@ -2570,12 +2570,12 @@
     <row r="116">
       <c r="B116" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D116" s="8" t="inlineStr">
         <is>
-          <t>1 Tim 5, 21.</t>
+          <t>In diesem Abschnitt des Briefes betont Bullinger seine Unvoreingenommenheit und die Bereitschaft zur Zusammenarbeit. Das Wort "praeiuditio" steht hier für Vorurteil oder Voreingenommenheit. Er drückt aus, dass seine Überlegungen und Absichten frei von persönlichen Vorurteilen sind. Angesichts ihrer gemeinsamen Anstrengungen unterstreicht er die Hoffnung auf das Beste, insbesondere im Hinblick auf die Zusammenarbeit mit Ambrosius Blarer und Simon Grynaeus. Diese Passage soll Vertrauen und Einigkeit in der theologischen Diskussion stärken.</t>
         </is>
       </c>
       <c r="E116" s="8" t="n"/>
@@ -2628,12 +2628,12 @@
     <row r="119">
       <c r="B119" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D119" s="8" t="inlineStr">
         <is>
-          <t>Eberardus a Rümlang, ein Zeitgenosse und Vermittler im Austausch zwischen Kunz und Bullinger, ist hier als vertrauenswürdiger Zeuge und Mittler dargestellt. Die Unterstützung und die Vertrauenswürdigkeit seiner Aussagen sollen jegliche Zweifel an Kunz' Absichten ausräumen.</t>
+          <t>Vgl. oben Nr. 1669, 2-36. 44-51; 1670, 17-25.</t>
         </is>
       </c>
       <c r="E119" s="8" t="n"/>
@@ -2644,12 +2644,12 @@
     <row r="120">
       <c r="B120" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D120" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Eberardus a Rümlang, ein Zeitgenosse und Vermittler im Austausch zwischen Kunz und Bullinger, ist hier als vertrauenswürdiger Zeuge und Mittler dargestellt. Die Unterstützung und die Vertrauenswürdigkeit seiner Aussagen sollen jegliche Zweifel an Kunz' Absichten ausräumen.</t>
         </is>
       </c>
       <c r="E120" s="7" t="n"/>
@@ -2660,12 +2660,12 @@
     <row r="121">
       <c r="B121" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D121" s="8" t="inlineStr">
         <is>
-          <t>Vgl. oben Nr. 1669, 2-36. 44-51; 1670, 17-25.</t>
+          <t>Gemeint ist: seit dem letzten brieflichen Kontakt im Jahr 1538 (s. &lt;bibl&gt;HBBW&lt;/bibl&gt; VIII, &lt;ref target="file11199"&gt;Nr. 1156&lt;/ref&gt;).</t>
         </is>
       </c>
       <c r="E121" s="8" t="n"/>
@@ -2697,7 +2697,7 @@
     <row r="123">
       <c r="B123" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="D123" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>&lt;p&gt;48. Digamię adsertores nit haben, eam apud christianos hodie in certis necessariis casibus licitam vel permittendam facere.</t>
         </is>
       </c>
       <c r="E123" s="7" t="n"/>
@@ -2734,7 +2734,7 @@
     <row r="125">
       <c r="B125" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D125" s="7" t="inlineStr">
@@ -2787,7 +2787,7 @@
     <row r="128">
       <c r="B128" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="D128" s="7" t="inlineStr">
         <is>
-          <t>Bullingers Vorhaben, die Vorrede seines Johanneskommentars von 1543 (HBBibl I 153) gesondert herauszugeben, wurde erst 1548 (HBBibl 1157) verwirklicht.</t>
+          <t>Oben &lt;ref target="file12260"&gt;Nr. 2213&lt;/ref&gt;, Anm. 4.</t>
         </is>
       </c>
       <c r="E128" s="7" t="n"/>
@@ -2808,12 +2808,12 @@
     <row r="129">
       <c r="B129" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D129" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Bullingers Vorhaben, die Vorrede seines Johanneskommentars von 1543 (HBBibl I 153) gesondert herauszugeben, wurde erst 1548 (HBBibl 1157) verwirklicht.</t>
         </is>
       </c>
       <c r="E129" s="8" t="n"/>
@@ -2824,7 +2824,7 @@
     <row r="130">
       <c r="B130" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D130" s="7" t="inlineStr">
@@ -2877,7 +2877,7 @@
     <row r="133">
       <c r="B133" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="D133" s="7" t="inlineStr">
         <is>
-          <t>Der erwähnte "pagus" könnte sich auf ein Dorf oder eine Landgemeinde in der Nähe von Straßburg beziehen, wohin Zwingli möglicherweise gebracht wurde, um abseits der städtischen Aufregung beerdigt zu werden. Es bleibt jedoch unklar, um welchen spezifischen Ort es sich handelt, da keine weiteren Details im Brief angegeben sind.</t>
+          <t>Zu verstehen: In eine andere Provinz.</t>
         </is>
       </c>
       <c r="E133" s="7" t="n"/>
@@ -2898,12 +2898,12 @@
     <row r="134">
       <c r="B134" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D134" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Nach Wasselnheim (Wasselonne, "Waßelen"; s. ebd.).</t>
         </is>
       </c>
       <c r="E134" s="8" t="n"/>
@@ -2914,12 +2914,12 @@
     <row r="135">
       <c r="B135" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D135" s="7" t="inlineStr">
         <is>
-          <t>Nach Wasselnheim (Wasselonne, "Waßelen"; s. ebd.).</t>
+          <t>Der erwähnte "pagus" könnte sich auf ein Dorf oder eine Landgemeinde in der Nähe von Straßburg beziehen, wohin Zwingli möglicherweise gebracht wurde, um abseits der städtischen Aufregung beerdigt zu werden. Es bleibt jedoch unklar, um welchen spezifischen Ort es sich handelt, da keine weiteren Details im Brief angegeben sind.</t>
         </is>
       </c>
       <c r="E135" s="7" t="n"/>
@@ -2967,7 +2967,7 @@
     <row r="138">
       <c r="B138" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="D138" s="7" t="inlineStr">
         <is>
-          <t>Zur Lage der Reformierten in Solothurn s. oben [Nr. 132] S. 237,3-19 und Haefliger 162-165.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E138" s="7" t="n"/>
@@ -2988,12 +2988,12 @@
     <row r="139">
       <c r="B139" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D139" s="8" t="inlineStr">
         <is>
-          <t>Die "Salodorenses pii" beziehen sich wahrscheinlich auf evangelische Christen aus der Region Solothurn. Zur damaligen Zeit war Solothurn eine katholische Stadt, und die Anhänger der Reformation mussten ihre Glaubensversammlungen heimlich oder in ländlichen Gebieten außerhalb der Stadt abhalten. Die Unterstützung, die sie einem Bruder für seine Predigt boten, wäre dabei von größter Wichtigkeit gewesen, um die reformatorischen Ideen zu verbreiten.</t>
+          <t>Die Saloderner, s. &lt;bibl&gt;HBLS&lt;/bibl&gt; II 6.</t>
         </is>
       </c>
       <c r="E139" s="8" t="n"/>
@@ -3004,12 +3004,12 @@
     <row r="140">
       <c r="B140" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D140" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Zur Lage der Reformierten in Solothurn s. oben [Nr. 132] S. 237,3-19 und Haefliger 162-165.</t>
         </is>
       </c>
       <c r="E140" s="7" t="n"/>
@@ -3020,12 +3020,12 @@
     <row r="141">
       <c r="B141" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D141" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Die "Salodorenses pii" beziehen sich wahrscheinlich auf evangelische Christen aus der Region Solothurn. Zur damaligen Zeit war Solothurn eine katholische Stadt, und die Anhänger der Reformation mussten ihre Glaubensversammlungen heimlich oder in ländlichen Gebieten außerhalb der Stadt abhalten. Die Unterstützung, die sie einem Bruder für seine Predigt boten, wäre dabei von größter Wichtigkeit gewesen, um die reformatorischen Ideen zu verbreiten.</t>
         </is>
       </c>
       <c r="E141" s="8" t="n"/>
@@ -3057,7 +3057,7 @@
     <row r="143">
       <c r="B143" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3067,7 +3067,7 @@
       </c>
       <c r="D143" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Myconius' Brief vom 5. Juli (Nr. 2943).</t>
         </is>
       </c>
       <c r="E143" s="7" t="n"/>
@@ -3078,12 +3078,12 @@
     <row r="144">
       <c r="B144" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D144" s="8" t="inlineStr">
         <is>
-          <t>Diese Formulierung deutet darauf hin, dass Bullinger entweder Briefe oder Nachrichten von Oswald Myconius durch eine Vermittlerin erhielt. In der Korrespondenz jener Zeit wurden oft Vertrauenspersonen für die sichere Zustellung von Briefen beauftragt. Der Kontext oder die Identität der Frau bleibt aus diesem Auszug jedoch unklar.</t>
+          <t>Unbekannt. - Zu dieser s. zuletzt &lt;ref target="file12992"&gt;Nr. 2943&lt;/ref&gt;,&lt;ptr target="qvzl17208-2" type="qv"/&gt;.</t>
         </is>
       </c>
       <c r="E144" s="8" t="n"/>
@@ -3094,12 +3094,12 @@
     <row r="145">
       <c r="B145" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D145" s="7" t="inlineStr">
         <is>
-          <t>Myconius' Brief vom 5. Juli (Nr. 2943).</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E145" s="7" t="n"/>
@@ -3110,12 +3110,12 @@
     <row r="146">
       <c r="B146" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D146" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Diese Formulierung deutet darauf hin, dass Bullinger entweder Briefe oder Nachrichten von Oswald Myconius durch eine Vermittlerin erhielt. In der Korrespondenz jener Zeit wurden oft Vertrauenspersonen für die sichere Zustellung von Briefen beauftragt. Der Kontext oder die Identität der Frau bleibt aus diesem Auszug jedoch unklar.</t>
         </is>
       </c>
       <c r="E146" s="8" t="n"/>
@@ -3147,7 +3147,7 @@
     <row r="148">
       <c r="B148" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D148" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Oben &lt;ref target="file11449"&gt;Nr. 1406&lt;/ref&gt; und 1411.</t>
         </is>
       </c>
       <c r="E148" s="7" t="n"/>
@@ -3168,12 +3168,12 @@
     <row r="149">
       <c r="B149" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D149" s="8" t="inlineStr">
         <is>
-          <t>Herzog Heinrich der Fromme, der Onkel der Landgräfin.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E149" s="8" t="n"/>
@@ -3184,12 +3184,12 @@
     <row r="150">
       <c r="B150" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D150" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Der Herzog von Sachsen, Johann Friedrich I., auch bekannt als Johann der Großmütige, war ein wichtiger protestantischer Anführer in den Schmalkaldischen Kriegen. Er galt als Unterstützer der Reformatoren Martin Luther und Philipp Melanchthon und hätte seinen Einfluss wahrscheinlich genutzt, um die Interessen und Ehren seiner Familienmitglieder und der protestantischen Sache zu verteidigen.</t>
         </is>
       </c>
       <c r="E150" s="7" t="n"/>
@@ -3200,12 +3200,12 @@
     <row r="151">
       <c r="B151" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D151" s="8" t="inlineStr">
         <is>
-          <t>Der Herzog von Sachsen, Johann Friedrich I., auch bekannt als Johann der Großmütige, war ein wichtiger protestantischer Anführer in den Schmalkaldischen Kriegen. Er galt als Unterstützer der Reformatoren Martin Luther und Philipp Melanchthon und hätte seinen Einfluss wahrscheinlich genutzt, um die Interessen und Ehren seiner Familienmitglieder und der protestantischen Sache zu verteidigen.</t>
+          <t>Herzog Heinrich der Fromme, der Onkel der Landgräfin.</t>
         </is>
       </c>
       <c r="E151" s="8" t="n"/>
@@ -3237,7 +3237,7 @@
     <row r="153">
       <c r="B153" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="D153" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Der Begriff „mansus“ bezeichnete im mittelalterlichen Rechtssystem einen landwirtschaftlichen Hof, der oft mit einer darauf befindlichen Villa verbunden war. Diese Begrifflichkeit ist typisch für das fränkische und alemannische Recht, wobei die genaue Definition und Nutzung im Laufe der Zeit variierten. Mansus wurde häufig als wirtschaftliche Einheit zur Berechnung von Abgaben und Dienstleistungen verwendet.</t>
         </is>
       </c>
       <c r="E153" s="7" t="n"/>
@@ -3258,12 +3258,12 @@
     <row r="154">
       <c r="B154" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D154" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>&lt;persName ref="p18532" cert="high"&gt;Iustiniani&lt;/persName&gt; aetas vocem raram et Graecam quidem &lt;foreign xml:lang="el"&gt;ἐµϕότευς&lt;/foreign&gt;&lt;note xml="fn19" type="footnote" n="19"&gt;&lt;/note&gt; frequentem fecit a verbo, arbitror, &lt;foreign xml:lang="el"&gt;ἐµϕυτεύω&lt;/foreign&gt;, quod „insero“ seu „implanto“ significat, quoniam eius generis locatione ager in familiae possessionem ita insertus et implantatus videri possit, ut avellare iure non liceat nisi pacto, ut diximus, locationis violato.</t>
         </is>
       </c>
       <c r="E154" s="8" t="n"/>
@@ -3274,12 +3274,12 @@
     <row r="155">
       <c r="B155" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D155" s="7" t="inlineStr">
         <is>
-          <t>Der Begriff „mansus“ bezeichnete im mittelalterlichen Rechtssystem einen landwirtschaftlichen Hof, der oft mit einer darauf befindlichen Villa verbunden war. Diese Begrifflichkeit ist typisch für das fränkische und alemannische Recht, wobei die genaue Definition und Nutzung im Laufe der Zeit variierten. Mansus wurde häufig als wirtschaftliche Einheit zur Berechnung von Abgaben und Dienstleistungen verwendet.</t>
+          <t>Zum Begriff "mansus" vgl. unten Anm. 27.</t>
         </is>
       </c>
       <c r="E155" s="7" t="n"/>
@@ -3290,12 +3290,12 @@
     <row r="156">
       <c r="B156" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D156" s="8" t="inlineStr">
         <is>
-          <t>Zum Begriff "mansus" vgl. unten Anm. 27.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E156" s="8" t="n"/>
@@ -3327,7 +3327,7 @@
     <row r="158">
       <c r="B158" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="D158" s="7" t="inlineStr">
         <is>
-          <t>In ihrer Protestation vom 4. August 1545 erneuerten die Stände der Augsburger Konfession ihre Forderungen bezüglich Friede und Recht und lehnten das Konzil von Trient ab; s. RTA JR XVI/2 1669-1672, Nr. 342.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E158" s="7" t="n"/>
@@ -3348,12 +3348,12 @@
     <row r="159">
       <c r="B159" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D159" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Siehe &lt;bibl&gt;Z&lt;/bibl&gt; 22.</t>
         </is>
       </c>
       <c r="E159" s="8" t="n"/>
@@ -3364,12 +3364,12 @@
     <row r="160">
       <c r="B160" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D160" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Diese Concessiones beziehen sich wahrscheinlich auf Zugeständnisse, die im Zuge der Verhandlungen auf Reichstagen gemacht wurden, insbesondere im Hinblick auf die religiösen und politischen Spannungen zwischen den katholischen und protestantischen Ständen im Heiligen Römischen Reich. Die Reformatoren kritisierten häufig die politischen Machenschaften, die zu ungunsten der protestantischen Sache geschahen.</t>
         </is>
       </c>
       <c r="E160" s="7" t="n"/>
@@ -3380,12 +3380,12 @@
     <row r="161">
       <c r="B161" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D161" s="8" t="inlineStr">
         <is>
-          <t>Diese Concessiones beziehen sich wahrscheinlich auf Zugeständnisse, die im Zuge der Verhandlungen auf Reichstagen gemacht wurden, insbesondere im Hinblick auf die religiösen und politischen Spannungen zwischen den katholischen und protestantischen Ständen im Heiligen Römischen Reich. Die Reformatoren kritisierten häufig die politischen Machenschaften, die zu ungunsten der protestantischen Sache geschahen.</t>
+          <t>In ihrer Protestation vom 4. August 1545 erneuerten die Stände der Augsburger Konfession ihre Forderungen bezüglich Friede und Recht und lehnten das Konzil von Trient ab; s. RTA JR XVI/2 1669-1672, Nr. 342.</t>
         </is>
       </c>
       <c r="E161" s="8" t="n"/>
@@ -3438,12 +3438,12 @@
     <row r="164">
       <c r="B164" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D164" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>In den vorausgegangenen Briefen &lt;persName ref="p1391" cert="high"&gt;Hallers&lt;/persName&gt; wird das hier behandelte Thema nicht erwähnt; möglicherweise ist ein Brief nicht erhalten.</t>
         </is>
       </c>
       <c r="E164" s="8" t="n"/>
@@ -3470,7 +3470,7 @@
     <row r="166">
       <c r="B166" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D166" s="8" t="inlineStr">
@@ -3507,7 +3507,7 @@
     <row r="168">
       <c r="B168" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="D168" s="7" t="inlineStr">
         <is>
-          <t>Das "Erblehen" (lat. Emphyteusis) beschreibt ein erbrechtliches Nutzungsverhältnis von Grundbesitz, bei dem der Empfänger das Land gegen einen vereinbarten Zins oder Verpflichtung dauerhaft nutzen kann. Dieses Rechtsinstitut war im Mittelalter weit verbreitet und ermöglichte es, Land langfristig zu bewirtschaften, ohne das Eigentum daran zu besitzen. Das Recht ging bei Erbschaft an die Nachkommen über, was es stabil und attraktiv für die Landwirtschaft und Siedlungsentwicklung machte.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E168" s="7" t="n"/>
@@ -3528,12 +3528,12 @@
     <row r="169">
       <c r="B169" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D169" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Das "Erblehen" (lat. Emphyteusis) beschreibt ein erbrechtliches Nutzungsverhältnis von Grundbesitz, bei dem der Empfänger das Land gegen einen vereinbarten Zins oder Verpflichtung dauerhaft nutzen kann. Dieses Rechtsinstitut war im Mittelalter weit verbreitet und ermöglichte es, Land langfristig zu bewirtschaften, ohne das Eigentum daran zu besitzen. Das Recht ging bei Erbschaft an die Nachkommen über, was es stabil und attraktiv für die Landwirtschaft und Siedlungsentwicklung machte.</t>
         </is>
       </c>
       <c r="E169" s="8" t="n"/>
@@ -3544,12 +3544,12 @@
     <row r="170">
       <c r="B170" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D170" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Zu den von Bullinger übersandten Urkunden und &lt;persName ref="p8049" cert="high"&gt;Vadians&lt;/persName&gt; autographen Urkundenübersetzungen vgl. unten die Beilage, Anm. 122,172 und 195.</t>
         </is>
       </c>
       <c r="E170" s="7" t="n"/>
@@ -3597,7 +3597,7 @@
     <row r="173">
       <c r="B173" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="D173" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Welcher Bruder von Jakob May gemeint ist, konnte nicht festgestellt werden.</t>
         </is>
       </c>
       <c r="E173" s="7" t="n"/>
@@ -3618,12 +3618,12 @@
     <row r="174">
       <c r="B174" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D174" s="8" t="inlineStr">
         <is>
-          <t>Welcher Bruder von Jakob May gemeint ist, konnte nicht festgestellt werden.</t>
+          <t>&lt;persName ref="p5789" cert="high"&gt;Jacob von Madis&lt;/persName&gt; Bruder.</t>
         </is>
       </c>
       <c r="E174" s="8" t="n"/>
@@ -3634,12 +3634,12 @@
     <row r="175">
       <c r="B175" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D175" s="7" t="inlineStr">
         <is>
-          <t>Unklar bleibt, welcher Jacobi a Madiis hier genau gemeint ist. Der Brief verweist jedoch auf eine engere Verbindung zwischen Bullinger und der Familie Madi, die in verschiedenen Funktionen in Zürich tätig waren. Siehe dazu auch Müller, „Die Zürcher Familie Madi und ihre Verbindungen“, in: Zürcher Jahrbuch für Regionalgeschichte, 1987, S. 145-160.</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E175" s="7" t="n"/>
@@ -3650,12 +3650,12 @@
     <row r="176">
       <c r="B176" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D176" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Unklar bleibt, welcher Jacobi a Madiis hier genau gemeint ist. Der Brief verweist jedoch auf eine engere Verbindung zwischen Bullinger und der Familie Madi, die in verschiedenen Funktionen in Zürich tätig waren. Siehe dazu auch Müller, „Die Zürcher Familie Madi und ihre Verbindungen“, in: Zürcher Jahrbuch für Regionalgeschichte, 1987, S. 145-160.</t>
         </is>
       </c>
       <c r="E176" s="8" t="n"/>
@@ -3687,7 +3687,7 @@
     <row r="178">
       <c r="B178" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="D178" s="7" t="inlineStr">
         <is>
-          <t>Vgl. dazu Bullingers Antwortbrief an Bucer, datiert auf den 20. Dezember 1534, in dem Bullinger auf die von Bucer erwähnte Confessio Bezug nimmt und seine Ansichten zur Abendmahlsfrage darlegt. (Siehe &lt;ref target="file10523"&gt;Nr. 476&lt;/ref&gt; in diesem Band.)</t>
+          <t>lorem ipsum dolor sit amet</t>
         </is>
       </c>
       <c r="E178" s="7" t="n"/>
@@ -3708,12 +3708,12 @@
     <row r="179">
       <c r="B179" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D179" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Vgl. dazu Bullingers Antwortbrief an Bucer, datiert auf den 20. Dezember 1534, in dem Bullinger auf die von Bucer erwähnte Confessio Bezug nimmt und seine Ansichten zur Abendmahlsfrage darlegt. (Siehe &lt;ref target="file10523"&gt;Nr. 476&lt;/ref&gt; in diesem Band.)</t>
         </is>
       </c>
       <c r="E179" s="8" t="n"/>
@@ -3724,12 +3724,12 @@
     <row r="180">
       <c r="B180" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D180" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Oben &lt;ref target="file10498"&gt;Nr. 463&lt;/ref&gt;, Anm. 31.</t>
         </is>
       </c>
       <c r="E180" s="7" t="n"/>
@@ -3777,7 +3777,7 @@
     <row r="183">
       <c r="B183" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3798,12 +3798,12 @@
     <row r="184">
       <c r="B184" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D184" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t xml:space="preserve">&lt;persName ref="p8127" cert="high"&gt;Pellikan&lt;/persName&gt; hatte im Jahre 1532 seine Kommentare zu den Schriften des Paulus veröffentlicht; s. &lt;bibl&gt;HBBW&lt;/bibl&gt; II 1. 7. 12. 25. 32. 34. 48. 56. 78. 82. 91. 95. 105. 114. 127. 130. 136. 139. 143. 148. 152. 155. 158. 161. 165. 168. 170. 173. 176. 179. 182. 185. 190. 193. 196. 199. 202. 205. 208. 211. 214. 218. 221. 225. 228. 231. 234. 237. 240. 244. 248. 251. 255. 258. 262. 265. 268. 272. 275. 278. 282. 285. 289. 292. 295. 299. 303. </t>
         </is>
       </c>
       <c r="E184" s="8" t="n"/>
@@ -3814,12 +3814,12 @@
     <row r="185">
       <c r="B185" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D185" s="7" t="inlineStr">
         <is>
-          <t>Zu Pellikans Kommentarwerk s. HBBW XII [Nr. 1646], S. 148f, Anm. 57.</t>
+          <t>Konrad Pellikan (1478–1556) war ein bedeutender Reformator und Hebräist, der in Zürich wirkte. Seine umfassende Arbeit an den "Kommentarien zu den Büchern der Bibel", die aus sieben Bänden bestand, prägte die reformatorische Bibelauslegung entscheidend. Pellikans detaillierte Kommentare galten als wertvolle Quelle für Theologen und Geistliche seiner Zeit.</t>
         </is>
       </c>
       <c r="E185" s="7" t="n"/>
@@ -3830,12 +3830,12 @@
     <row r="186">
       <c r="B186" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D186" s="8" t="inlineStr">
         <is>
-          <t>Konrad Pellikan (1478–1556) war ein bedeutender Reformator und Hebräist, der in Zürich wirkte. Seine umfassende Arbeit an den "Kommentarien zu den Büchern der Bibel", die aus sieben Bänden bestand, prägte die reformatorische Bibelauslegung entscheidend. Pellikans detaillierte Kommentare galten als wertvolle Quelle für Theologen und Geistliche seiner Zeit.</t>
+          <t>Zu Pellikans Kommentarwerk s. HBBW XII [Nr. 1646], S. 148f, Anm. 57.</t>
         </is>
       </c>
       <c r="E186" s="8" t="n"/>
@@ -3867,7 +3867,7 @@
     <row r="188">
       <c r="B188" t="inlineStr">
         <is>
-          <t>text_footnote</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -3877,7 +3877,7 @@
       </c>
       <c r="D188" s="7" t="inlineStr">
         <is>
-          <t>Johannes und Justus Vulteius.</t>
+          <t>Die zwei erwähnten Jugendlichen könnten Studenten oder Lehrlinge gewesen sein, die von Marburg nach Zürich reisten. Eine genauere Identifikation ist ohne zusätzliche Quellen schwierig. Eventuell handelt es sich um Theologiestudenten, die bei Heinrich Bullinger studieren oder sich ausbilden lassen wollten.</t>
         </is>
       </c>
       <c r="E188" s="7" t="n"/>
@@ -3888,12 +3888,12 @@
     <row r="189">
       <c r="B189" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>text_footnote</t>
         </is>
       </c>
       <c r="D189" s="8" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Johannes und Justus Vulteius.</t>
         </is>
       </c>
       <c r="E189" s="8" t="n"/>
@@ -3904,7 +3904,7 @@
     <row r="190">
       <c r="B190" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D190" s="7" t="inlineStr">
@@ -3920,12 +3920,12 @@
     <row r="191">
       <c r="B191" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D191" s="8" t="inlineStr">
         <is>
-          <t>Die zwei erwähnten Jugendlichen könnten Studenten oder Lehrlinge gewesen sein, die von Marburg nach Zürich reisten. Eine genauere Identifikation ist ohne zusätzliche Quellen schwierig. Eventuell handelt es sich um Theologiestudenten, die bei Heinrich Bullinger studieren oder sich ausbilden lassen wollten.</t>
+          <t>Die beiden Brüder; s. unten.</t>
         </is>
       </c>
       <c r="E191" s="8" t="n"/>
@@ -3957,7 +3957,7 @@
     <row r="193">
       <c r="B193" t="inlineStr">
         <is>
-          <t>fake_model2</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="D193" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>&lt;persName ref="p18118" cert="high"&gt;Philippa von Hessen&lt;/persName&gt;.</t>
         </is>
       </c>
       <c r="E193" s="7" t="n"/>
@@ -3994,7 +3994,7 @@
     <row r="195">
       <c r="B195" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>fake_model2</t>
         </is>
       </c>
       <c r="D195" s="7" t="inlineStr">
@@ -4084,12 +4084,12 @@
     <row r="200">
       <c r="B200" t="inlineStr">
         <is>
-          <t>fake_model1</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D200" s="7" t="inlineStr">
         <is>
-          <t>lorem ipsum dolor sit amet</t>
+          <t>Die Erwähnung einer "altera" bezieht sich vermutlich auf eine weitere im Brief erwähnte Person im Umfeld des Landgrafen von Hessen. In diesem Kontext ist es möglich, dass "altera" auf eine andere Geliebte oder sogar Ehefrau bezogen ist, was im historischen Hintergrund der Landgrafen von Hessen, insbesondere im Zusammenhang mit landgräflichen Familienstreitigkeiten und der komplexen Heiratspolitik, nicht selten war. Eine detaillierte Identifizierung erfordert jedoch umfassendere historische Recherchen in den familiären Verflechtungen des Landgrafenhofes dieser Zeit.</t>
         </is>
       </c>
       <c r="E200" s="7" t="n"/>
@@ -4100,12 +4100,12 @@
     <row r="201">
       <c r="B201" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>llama-8B</t>
         </is>
       </c>
       <c r="D201" s="8" t="inlineStr">
         <is>
-          <t>Die Erwähnung einer "altera" bezieht sich vermutlich auf eine weitere im Brief erwähnte Person im Umfeld des Landgrafen von Hessen. In diesem Kontext ist es möglich, dass "altera" auf eine andere Geliebte oder sogar Ehefrau bezogen ist, was im historischen Hintergrund der Landgrafen von Hessen, insbesondere im Zusammenhang mit landgräflichen Familienstreitigkeiten und der komplexen Heiratspolitik, nicht selten war. Eine detaillierte Identifizierung erfordert jedoch umfassendere historische Recherchen in den familiären Verflechtungen des Landgrafenhofes dieser Zeit.</t>
+          <t>&lt;persName ref="p4141" cert="high"&gt;Rodolphus Ryff&lt;/persName&gt;.</t>
         </is>
       </c>
       <c r="E201" s="8" t="n"/>

</xml_diff>